<commit_message>
Added latitude and longitute to papers.csv, as well as minor edits
I found the latitude and longitude for every study site and included it
in papers.csv. I used decimal degrees.

For papers that reported data from multiple sites, I added an extra
column for every additional site.

I also made a few minor edits to the data extraction workbook and
decisions.csv.
</commit_message>
<xml_diff>
--- a/Data Extraction Workbook/Copy of Excel Calculator for Means of means and SE's ONLY USED PAPERS.xlsx
+++ b/Data Extraction Workbook/Copy of Excel Calculator for Means of means and SE's ONLY USED PAPERS.xlsx
@@ -288,9 +288,6 @@
     <t>F.Conrol</t>
   </si>
   <si>
-    <t>Kerns</t>
-  </si>
-  <si>
     <t>Huffman</t>
   </si>
   <si>
@@ -367,6 +364,9 @@
   </si>
   <si>
     <t>RiparianLowSeverity</t>
+  </si>
+  <si>
+    <t>Kerns+Thies+etal-2006</t>
   </si>
 </sst>
 </file>
@@ -521,15 +521,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>88446</xdr:colOff>
+          <xdr:colOff>83004</xdr:colOff>
           <xdr:row>94</xdr:row>
-          <xdr:rowOff>63954</xdr:rowOff>
+          <xdr:rowOff>69396</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>240846</xdr:colOff>
+          <xdr:colOff>302079</xdr:colOff>
           <xdr:row>95</xdr:row>
-          <xdr:rowOff>48986</xdr:rowOff>
+          <xdr:rowOff>108857</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -562,15 +562,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>88446</xdr:colOff>
+          <xdr:colOff>83004</xdr:colOff>
           <xdr:row>94</xdr:row>
-          <xdr:rowOff>63954</xdr:rowOff>
+          <xdr:rowOff>69396</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>240846</xdr:colOff>
+          <xdr:colOff>302079</xdr:colOff>
           <xdr:row>95</xdr:row>
-          <xdr:rowOff>48986</xdr:rowOff>
+          <xdr:rowOff>108857</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -891,8 +891,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AR539"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A471" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A502" sqref="A502"/>
+    <sheetView tabSelected="1" topLeftCell="A269" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A297" sqref="A297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -903,12 +903,12 @@
     <col min="14" max="14" width="9.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" ht="15">
+    <row r="1" spans="1:44">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:44" ht="15">
+    <row r="2" spans="1:44">
       <c r="A2" s="4" t="s">
         <v>32</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="AQ3" s="1"/>
       <c r="AR3" s="1"/>
     </row>
-    <row r="4" spans="1:44" ht="15">
+    <row r="4" spans="1:44">
       <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="5" spans="1:44" ht="15">
+    <row r="5" spans="1:44">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -1148,7 +1148,7 @@
       <c r="AQ5" s="2"/>
       <c r="AR5" s="2"/>
     </row>
-    <row r="6" spans="1:44" ht="15">
+    <row r="6" spans="1:44">
       <c r="A6" s="5" t="s">
         <v>21</v>
       </c>
@@ -1288,7 +1288,7 @@
       <c r="AQ7" s="3"/>
       <c r="AR7" s="3"/>
     </row>
-    <row r="8" spans="1:44" ht="15">
+    <row r="8" spans="1:44">
       <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
@@ -5588,7 +5588,7 @@
     </row>
     <row r="210" spans="1:19">
       <c r="A210" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="211" spans="1:19">
@@ -5629,7 +5629,7 @@
         <v>43</v>
       </c>
       <c r="M211" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N211" t="s">
         <v>16</v>
@@ -5960,7 +5960,7 @@
         <v>43</v>
       </c>
       <c r="M217" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N217" t="s">
         <v>16</v>
@@ -7707,7 +7707,7 @@
     </row>
     <row r="283" spans="1:33">
       <c r="A283" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AB283" s="9"/>
       <c r="AE283" s="9"/>
@@ -7819,7 +7819,7 @@
         <v>3</v>
       </c>
       <c r="D290" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E290" s="2"/>
       <c r="F290" s="2"/>
@@ -7973,7 +7973,7 @@
     </row>
     <row r="296" spans="1:33">
       <c r="A296" s="8" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="C296" s="6"/>
       <c r="D296" s="6"/>
@@ -8274,7 +8274,7 @@
         <v>1</v>
       </c>
       <c r="C303" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E303">
         <v>1.7161999999999999</v>
@@ -8531,7 +8531,7 @@
     </row>
     <row r="310" spans="1:33">
       <c r="A310" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C310" s="6"/>
       <c r="D310" s="6"/>
@@ -9011,7 +9011,7 @@
     </row>
     <row r="324" spans="1:13">
       <c r="A324" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="325" spans="1:13">
@@ -9141,12 +9141,12 @@
     </row>
     <row r="338" spans="1:7">
       <c r="A338" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="339" spans="1:7">
       <c r="A339" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="340" spans="1:7">
@@ -9344,7 +9344,7 @@
     </row>
     <row r="353" spans="1:10">
       <c r="A353" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C353" s="11"/>
     </row>
@@ -9544,7 +9544,7 @@
     </row>
     <row r="367" spans="1:10">
       <c r="A367" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C367" s="6"/>
       <c r="D367" s="6"/>
@@ -9611,7 +9611,7 @@
       <c r="I370" s="6"/>
       <c r="J370" s="2"/>
       <c r="M370" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="371" spans="1:13" ht="15">
@@ -9666,7 +9666,7 @@
     </row>
     <row r="374" spans="1:13" ht="15">
       <c r="A374" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B374" s="12"/>
       <c r="H374" s="6"/>
@@ -10006,7 +10006,7 @@
     </row>
     <row r="397" spans="1:9">
       <c r="A397" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="398" spans="1:9">
@@ -10162,13 +10162,13 @@
     </row>
     <row r="408" spans="1:14">
       <c r="A408" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C408" s="6"/>
     </row>
     <row r="409" spans="1:14">
       <c r="A409" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C409" s="6"/>
     </row>
@@ -10192,7 +10192,7 @@
         <v>43</v>
       </c>
       <c r="G410" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="411" spans="1:14" ht="15">
@@ -10277,7 +10277,7 @@
         <v>0.28284271247461906</v>
       </c>
       <c r="D414">
-        <f t="shared" ref="D414:G414" si="36">(SQRT(D411-1))*D413</f>
+        <f t="shared" ref="D414" si="36">(SQRT(D411-1))*D413</f>
         <v>0.28284271247461906</v>
       </c>
       <c r="E414">
@@ -10311,7 +10311,7 @@
         <v>43</v>
       </c>
       <c r="D415" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E415" s="1"/>
     </row>
@@ -10378,7 +10378,7 @@
     </row>
     <row r="420" spans="1:7">
       <c r="A420" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C420" s="6"/>
     </row>
@@ -10402,7 +10402,7 @@
         <v>43</v>
       </c>
       <c r="G421" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="422" spans="1:7" ht="15">
@@ -10487,7 +10487,7 @@
         <v>0.28284271247461906</v>
       </c>
       <c r="D425">
-        <f t="shared" ref="D425:G425" si="39">(SQRT(D422-1))*D424</f>
+        <f t="shared" ref="D425" si="39">(SQRT(D422-1))*D424</f>
         <v>0.42426406871192851</v>
       </c>
       <c r="E425">
@@ -10514,7 +10514,7 @@
         <v>43</v>
       </c>
       <c r="D426" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E426" s="6"/>
     </row>
@@ -10580,7 +10580,7 @@
     </row>
     <row r="431" spans="1:7" ht="15">
       <c r="A431" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B431" s="1"/>
       <c r="C431" s="1"/>
@@ -10704,10 +10704,10 @@
     </row>
     <row r="442" spans="1:7">
       <c r="A442" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B442" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="443" spans="1:7">
@@ -10724,7 +10724,7 @@
         <v>63</v>
       </c>
       <c r="E443" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F443" t="s">
         <v>41</v>
@@ -10912,7 +10912,7 @@
         <v>0</v>
       </c>
       <c r="C452">
-        <f t="shared" ref="C452:G452" si="46">(SQRT(C449-1))*C451</f>
+        <f t="shared" ref="C452:E452" si="46">(SQRT(C449-1))*C451</f>
         <v>0</v>
       </c>
       <c r="D452">
@@ -10926,7 +10926,7 @@
     </row>
     <row r="453" spans="1:15">
       <c r="A453" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="454" spans="1:15">
@@ -11026,7 +11026,7 @@
     </row>
     <row r="459" spans="1:15" ht="15">
       <c r="A459" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B459" s="1"/>
       <c r="C459" s="1"/>
@@ -11045,7 +11045,7 @@
     </row>
     <row r="460" spans="1:15" ht="15">
       <c r="A460" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="461" spans="1:15">
@@ -11163,7 +11163,7 @@
     </row>
     <row r="466" spans="1:5" ht="15">
       <c r="A466" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="467" spans="1:5">
@@ -11225,7 +11225,7 @@
     </row>
     <row r="472" spans="1:5" ht="15">
       <c r="A472" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="473" spans="1:5">
@@ -11287,7 +11287,7 @@
     </row>
     <row r="478" spans="1:5" ht="15">
       <c r="A478" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="479" spans="1:5">
@@ -11349,7 +11349,7 @@
     </row>
     <row r="484" spans="1:3" ht="15">
       <c r="A484" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="485" spans="1:3">
@@ -11411,7 +11411,7 @@
     </row>
     <row r="490" spans="1:3" ht="15">
       <c r="A490" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="491" spans="1:3">
@@ -11473,7 +11473,7 @@
     </row>
     <row r="496" spans="1:3" ht="15">
       <c r="A496" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="497" spans="1:3">
@@ -11655,52 +11655,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId4" name="Control 2">
-          <controlPr defaultSize="0" r:id="rId5">
+        <control shapeId="1025" r:id="rId4" name="Control 1">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>85725</xdr:colOff>
-                <xdr:row>94</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
+                <xdr:colOff>76200</xdr:colOff>
+                <xdr:row>95</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>238125</xdr:colOff>
-                <xdr:row>95</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>295275</xdr:colOff>
+                <xdr:row>97</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId4" name="Control 2"/>
+        <control shapeId="1025" r:id="rId4" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId6" name="Control 1">
-          <controlPr defaultSize="0" r:id="rId5">
+        <control shapeId="1026" r:id="rId6" name="Control 2">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>85725</xdr:colOff>
-                <xdr:row>94</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
+                <xdr:colOff>76200</xdr:colOff>
+                <xdr:row>95</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>238125</xdr:colOff>
-                <xdr:row>95</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>295275</xdr:colOff>
+                <xdr:row>97</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId6" name="Control 1"/>
+        <control shapeId="1026" r:id="rId6" name="Control 2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Added FireSeverity to papers.csv, and minor edits/housekeeping on other documents
I pulled fire severity data from each paper with burn treatments.

At present, this data needs additional editing, and I need to ask
questions about the fire severities.

Housekeeping: I also cleaned up some of the data files in response-vars,
and added a few papers that had not been added yet. I also cleaned up my
Data Extraction Workbook.
</commit_message>
<xml_diff>
--- a/Data Extraction Workbook/Copy of Excel Calculator for Means of means and SE's ONLY USED PAPERS.xlsx
+++ b/Data Extraction Workbook/Copy of Excel Calculator for Means of means and SE's ONLY USED PAPERS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="285" windowWidth="8310" windowHeight="2505"/>
+    <workbookView xWindow="16335" yWindow="345" windowWidth="12330" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -466,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -489,6 +489,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,15 +522,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>83004</xdr:colOff>
-          <xdr:row>94</xdr:row>
-          <xdr:rowOff>69396</xdr:rowOff>
+          <xdr:colOff>69396</xdr:colOff>
+          <xdr:row>97</xdr:row>
+          <xdr:rowOff>81643</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>302079</xdr:colOff>
-          <xdr:row>95</xdr:row>
-          <xdr:rowOff>108857</xdr:rowOff>
+          <xdr:colOff>221796</xdr:colOff>
+          <xdr:row>98</xdr:row>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -562,15 +563,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>83004</xdr:colOff>
-          <xdr:row>94</xdr:row>
-          <xdr:rowOff>69396</xdr:rowOff>
+          <xdr:colOff>69396</xdr:colOff>
+          <xdr:row>97</xdr:row>
+          <xdr:rowOff>81643</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>302079</xdr:colOff>
-          <xdr:row>95</xdr:row>
-          <xdr:rowOff>108857</xdr:rowOff>
+          <xdr:colOff>221796</xdr:colOff>
+          <xdr:row>98</xdr:row>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -891,8 +892,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AR539"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A269" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A297" sqref="A297"/>
+    <sheetView tabSelected="1" topLeftCell="A360" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D396" sqref="D396"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1214,75 +1215,75 @@
         <v>0</v>
       </c>
       <c r="B7" s="3">
-        <f t="shared" ref="B7:S7" si="0">AVERAGE(B4:B6)</f>
+        <f>AVERAGE(B4:B6)</f>
         <v>52.6</v>
       </c>
       <c r="C7" s="3">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(C4:C6)</f>
         <v>59.933333333333337</v>
       </c>
       <c r="D7" s="3">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D4:D6)</f>
         <v>50.966666666666661</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(E4:E6)</f>
         <v>48.79999999999999</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(F4:F6)</f>
         <v>53.9</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(G4:G6)</f>
         <v>46.533333333333339</v>
       </c>
       <c r="H7" s="3">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(H4:H6)</f>
         <v>3.7000000000000006</v>
       </c>
       <c r="I7" s="3">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(I4:I6)</f>
         <v>5.9666666666666659</v>
       </c>
       <c r="J7" s="3">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(J4:J6)</f>
         <v>4.3666666666666663</v>
       </c>
       <c r="K7" s="3">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(K4:K6)</f>
         <v>11.166666666666666</v>
       </c>
       <c r="L7" s="3">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(L4:L6)</f>
         <v>12.533333333333333</v>
       </c>
       <c r="M7" s="3">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(M4:M6)</f>
         <v>9.7000000000000011</v>
       </c>
       <c r="N7" s="3">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(N4:N6)</f>
         <v>30.666666666666668</v>
       </c>
       <c r="O7" s="3">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O4:O6)</f>
         <v>35.266666666666673</v>
       </c>
       <c r="P7" s="3">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(P4:P6)</f>
         <v>31.8</v>
       </c>
       <c r="Q7" s="3">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(Q4:Q6)</f>
         <v>8.6333333333333346</v>
       </c>
       <c r="R7" s="3">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(R4:R6)</f>
         <v>9.8000000000000007</v>
       </c>
       <c r="S7" s="3">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(S4:S6)</f>
         <v>7.3666666666666671</v>
       </c>
       <c r="AQ7" s="3"/>
@@ -1476,75 +1477,75 @@
         <v>27</v>
       </c>
       <c r="B11" s="3">
-        <f t="shared" ref="B11:S11" si="1">AVERAGE(B8:B10)</f>
+        <f>AVERAGE(B8:B10)</f>
         <v>2.0666666666666669</v>
       </c>
       <c r="C11" s="3">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(C8:C10)</f>
         <v>4.0666666666666664</v>
       </c>
       <c r="D11" s="3">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D8:D10)</f>
         <v>5.3666666666666671</v>
       </c>
       <c r="E11" s="3">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(E8:E10)</f>
         <v>1.1666666666666667</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(F8:F10)</f>
         <v>2.9333333333333336</v>
       </c>
       <c r="G11" s="3">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(G8:G10)</f>
         <v>4.1000000000000005</v>
       </c>
       <c r="H11" s="3">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(H8:H10)</f>
         <v>0.9</v>
       </c>
       <c r="I11" s="3">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(I8:I10)</f>
         <v>1.1333333333333333</v>
       </c>
       <c r="J11" s="3">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(J8:J10)</f>
         <v>1.3666666666666665</v>
       </c>
       <c r="K11" s="3">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(K8:K10)</f>
         <v>1.4666666666666668</v>
       </c>
       <c r="L11" s="3">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(L8:L10)</f>
         <v>1</v>
       </c>
       <c r="M11" s="3">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(M8:M10)</f>
         <v>1.7</v>
       </c>
       <c r="N11" s="3">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(N8:N10)</f>
         <v>0.93333333333333324</v>
       </c>
       <c r="O11" s="3">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O8:O10)</f>
         <v>2.0666666666666664</v>
       </c>
       <c r="P11" s="3">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(P8:P10)</f>
         <v>3.1999999999999997</v>
       </c>
       <c r="Q11" s="3">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(Q8:Q10)</f>
         <v>0.93333333333333324</v>
       </c>
       <c r="R11" s="3">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(R8:R10)</f>
         <v>1.1666666666666667</v>
       </c>
       <c r="S11" s="3">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(S8:S10)</f>
         <v>0.76666666666666661</v>
       </c>
       <c r="AQ11" s="3"/>
@@ -1555,75 +1556,75 @@
         <v>25</v>
       </c>
       <c r="B12" s="6">
-        <f t="shared" ref="B12:S12" si="2">(SQRT(B3-1))*B11</f>
+        <f>(SQRT(B3-1))*B11</f>
         <v>2.9227080289043967</v>
       </c>
       <c r="C12" s="6">
-        <f t="shared" si="2"/>
+        <f>(SQRT(C3-1))*C11</f>
         <v>5.751135153650587</v>
       </c>
       <c r="D12" s="6">
-        <f t="shared" si="2"/>
+        <f>(SQRT(D3-1))*D11</f>
         <v>7.5896127847356114</v>
       </c>
       <c r="E12" s="6">
-        <f t="shared" si="2"/>
+        <f>(SQRT(E3-1))*E11</f>
         <v>1.649915822768611</v>
       </c>
       <c r="F12" s="6">
-        <f t="shared" si="2"/>
+        <f>(SQRT(F3-1))*F11</f>
         <v>4.1483597829610792</v>
       </c>
       <c r="G12" s="6">
-        <f t="shared" si="2"/>
+        <f>(SQRT(G3-1))*G11</f>
         <v>5.7982756057296907</v>
       </c>
       <c r="H12" s="6">
-        <f t="shared" si="2"/>
+        <f>(SQRT(H3-1))*H11</f>
         <v>1.2727922061357857</v>
       </c>
       <c r="I12" s="6">
-        <f t="shared" si="2"/>
+        <f>(SQRT(I3-1))*I11</f>
         <v>1.6027753706895078</v>
       </c>
       <c r="J12" s="6">
-        <f t="shared" si="2"/>
+        <f>(SQRT(J3-1))*J11</f>
         <v>1.9327585352432297</v>
       </c>
       <c r="K12" s="6">
-        <f t="shared" si="2"/>
+        <f>(SQRT(K3-1))*K11</f>
         <v>2.0741798914805396</v>
       </c>
       <c r="L12" s="6">
-        <f t="shared" si="2"/>
+        <f>(SQRT(L3-1))*L11</f>
         <v>1.4142135623730951</v>
       </c>
       <c r="M12" s="6">
-        <f t="shared" si="2"/>
+        <f>(SQRT(M3-1))*M11</f>
         <v>2.4041630560342617</v>
       </c>
       <c r="N12" s="6">
-        <f t="shared" si="2"/>
+        <f>(SQRT(N3-1))*N11</f>
         <v>1.3199326582148887</v>
       </c>
       <c r="O12" s="6">
-        <f t="shared" si="2"/>
+        <f>(SQRT(O3-1))*O11</f>
         <v>2.9227080289043963</v>
       </c>
       <c r="P12" s="6">
-        <f t="shared" si="2"/>
+        <f>(SQRT(P3-1))*P11</f>
         <v>4.5254833995939041</v>
       </c>
       <c r="Q12" s="6">
-        <f t="shared" si="2"/>
+        <f>(SQRT(Q3-1))*Q11</f>
         <v>1.3199326582148887</v>
       </c>
       <c r="R12" s="6">
-        <f t="shared" si="2"/>
+        <f>(SQRT(R3-1))*R11</f>
         <v>1.649915822768611</v>
       </c>
       <c r="S12" s="6">
-        <f t="shared" si="2"/>
+        <f>(SQRT(S3-1))*S11</f>
         <v>1.0842303978193728</v>
       </c>
       <c r="AQ12" s="6"/>
@@ -2066,75 +2067,75 @@
         <v>0</v>
       </c>
       <c r="B21" s="3">
-        <f t="shared" ref="B21:S21" si="3">AVERAGE(B18:B20)</f>
+        <f>AVERAGE(B18:B20)</f>
         <v>25.166666666666668</v>
       </c>
       <c r="C21" s="3">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(C18:C20)</f>
         <v>27.400000000000002</v>
       </c>
       <c r="D21" s="3">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(D18:D20)</f>
         <v>19.7</v>
       </c>
       <c r="E21" s="3">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(E18:E20)</f>
         <v>24.899999999999995</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(F18:F20)</f>
         <v>26.966666666666669</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(G18:G20)</f>
         <v>19.333333333333332</v>
       </c>
       <c r="H21" s="3">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(H18:H20)</f>
         <v>0.23333333333333331</v>
       </c>
       <c r="I21" s="3">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(I18:I20)</f>
         <v>0.46666666666666662</v>
       </c>
       <c r="J21" s="3">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(J18:J20)</f>
         <v>0.3666666666666667</v>
       </c>
       <c r="K21" s="3">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(K18:K20)</f>
         <v>2.7666666666666671</v>
       </c>
       <c r="L21" s="3">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(L18:L20)</f>
         <v>3</v>
       </c>
       <c r="M21" s="3">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(M18:M20)</f>
         <v>2.1333333333333333</v>
       </c>
       <c r="N21" s="3">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(N18:N20)</f>
         <v>10.6</v>
       </c>
       <c r="O21" s="3">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(O18:O20)</f>
         <v>11.300000000000002</v>
       </c>
       <c r="P21" s="3">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(P18:P20)</f>
         <v>8.6</v>
       </c>
       <c r="Q21" s="3">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(Q18:Q20)</f>
         <v>10.5</v>
       </c>
       <c r="R21" s="3">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(R18:R20)</f>
         <v>12.033333333333333</v>
       </c>
       <c r="S21" s="3">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(S18:S20)</f>
         <v>8.25</v>
       </c>
     </row>
@@ -2320,75 +2321,75 @@
         <v>27</v>
       </c>
       <c r="B25" s="3">
-        <f t="shared" ref="B25:S25" si="4">AVERAGE(B22:B24)</f>
+        <f>AVERAGE(B22:B24)</f>
         <v>2.5333333333333337</v>
       </c>
       <c r="C25" s="3">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(C22:C24)</f>
         <v>1.1333333333333331</v>
       </c>
       <c r="D25" s="3">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(D22:D24)</f>
         <v>1.5</v>
       </c>
       <c r="E25" s="3">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(E22:E24)</f>
         <v>2.5333333333333337</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(F22:F24)</f>
         <v>1.1333333333333335</v>
       </c>
       <c r="G25" s="3">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(G22:G24)</f>
         <v>1.3666666666666665</v>
       </c>
       <c r="H25" s="3">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(H22:H24)</f>
         <v>0.10000000000000002</v>
       </c>
       <c r="I25" s="3">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(I22:I24)</f>
         <v>0.23333333333333331</v>
       </c>
       <c r="J25" s="3">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(J22:J24)</f>
         <v>0.23333333333333331</v>
       </c>
       <c r="K25" s="3">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(K22:K24)</f>
         <v>0.3</v>
       </c>
       <c r="L25" s="3">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(L22:L24)</f>
         <v>0.26666666666666666</v>
       </c>
       <c r="M25" s="3">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(M22:M24)</f>
         <v>0.10000000000000002</v>
       </c>
       <c r="N25" s="3">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(N22:N24)</f>
         <v>1.8666666666666665</v>
       </c>
       <c r="O25" s="3">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(O22:O24)</f>
         <v>0.39999999999999997</v>
       </c>
       <c r="P25" s="3">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(P22:P24)</f>
         <v>1.0333333333333334</v>
       </c>
       <c r="Q25" s="3">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(Q22:Q24)</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="R25" s="3">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(R22:R24)</f>
         <v>0.9</v>
       </c>
       <c r="S25" s="3">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(S22:S24)</f>
         <v>0.6333333333333333</v>
       </c>
     </row>
@@ -2397,75 +2398,75 @@
         <v>25</v>
       </c>
       <c r="B26" s="6">
-        <f t="shared" ref="B26:S26" si="5">(SQRT(B17-1))*B25</f>
+        <f>(SQRT(B17-1))*B25</f>
         <v>3.5826743580118414</v>
       </c>
       <c r="C26" s="6">
-        <f t="shared" si="5"/>
+        <f>(SQRT(C17-1))*C25</f>
         <v>1.6027753706895074</v>
       </c>
       <c r="D26" s="6">
-        <f t="shared" si="5"/>
+        <f>(SQRT(D17-1))*D25</f>
         <v>2.1213203435596428</v>
       </c>
       <c r="E26" s="6">
-        <f t="shared" si="5"/>
+        <f>(SQRT(E17-1))*E25</f>
         <v>3.5826743580118414</v>
       </c>
       <c r="F26" s="6">
-        <f t="shared" si="5"/>
+        <f>(SQRT(F17-1))*F25</f>
         <v>1.602775370689508</v>
       </c>
       <c r="G26" s="6">
-        <f t="shared" si="5"/>
+        <f>(SQRT(G17-1))*G25</f>
         <v>1.9327585352432297</v>
       </c>
       <c r="H26" s="6">
-        <f t="shared" si="5"/>
+        <f>(SQRT(H17-1))*H25</f>
         <v>0.14142135623730953</v>
       </c>
       <c r="I26" s="6">
-        <f t="shared" si="5"/>
+        <f>(SQRT(I17-1))*I25</f>
         <v>0.32998316455372217</v>
       </c>
       <c r="J26" s="6">
-        <f t="shared" si="5"/>
+        <f>(SQRT(J17-1))*J25</f>
         <v>0.32998316455372217</v>
       </c>
       <c r="K26" s="6">
-        <f t="shared" si="5"/>
+        <f>(SQRT(K17-1))*K25</f>
         <v>0.42426406871192851</v>
       </c>
       <c r="L26" s="6">
-        <f t="shared" si="5"/>
+        <f>(SQRT(L17-1))*L25</f>
         <v>0.37712361663282534</v>
       </c>
       <c r="M26" s="6">
-        <f t="shared" si="5"/>
+        <f>(SQRT(M17-1))*M25</f>
         <v>0.14142135623730953</v>
       </c>
       <c r="N26" s="6">
-        <f t="shared" si="5"/>
+        <f>(SQRT(N17-1))*N25</f>
         <v>2.6398653164297774</v>
       </c>
       <c r="O26" s="6">
-        <f t="shared" si="5"/>
+        <f>(SQRT(O17-1))*O25</f>
         <v>0.56568542494923801</v>
       </c>
       <c r="P26" s="6">
-        <f t="shared" si="5"/>
+        <f>(SQRT(P17-1))*P25</f>
         <v>1.4613540144521984</v>
       </c>
       <c r="Q26" s="6">
-        <f t="shared" si="5"/>
+        <f>(SQRT(Q17-1))*Q25</f>
         <v>1.5556349186104048</v>
       </c>
       <c r="R26" s="6">
-        <f t="shared" si="5"/>
+        <f>(SQRT(R17-1))*R25</f>
         <v>1.2727922061357857</v>
       </c>
       <c r="S26" s="6">
-        <f t="shared" si="5"/>
+        <f>(SQRT(S17-1))*S25</f>
         <v>0.89566858950296024</v>
       </c>
     </row>
@@ -2706,27 +2707,27 @@
         <v>25</v>
       </c>
       <c r="B35">
-        <f t="shared" ref="B35:G35" si="6">(SQRT(B32-1))*B34</f>
+        <f t="shared" ref="B35:G35" si="0">(SQRT(B32-1))*B34</f>
         <v>0.62225396744416184</v>
       </c>
       <c r="C35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>1.2586500705120547</v>
       </c>
       <c r="D35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>1.2586500705120547</v>
       </c>
       <c r="E35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>0.94328044610285455</v>
       </c>
       <c r="F35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>1.2586500705120547</v>
       </c>
       <c r="G35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>1.8809040379562167</v>
       </c>
     </row>
@@ -2995,59 +2996,59 @@
         <v>3.1112698372208096</v>
       </c>
       <c r="C44">
-        <f t="shared" ref="C44:P44" si="7">(SQRT(C41-1))*C43</f>
+        <f t="shared" ref="C44:P44" si="1">(SQRT(C41-1))*C43</f>
         <v>4.3840620433565949</v>
       </c>
       <c r="D44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>0.98994949366116658</v>
       </c>
       <c r="E44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>0.98994949366116658</v>
       </c>
       <c r="F44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>1.9798989873223332</v>
       </c>
       <c r="G44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>0.98994949366116658</v>
       </c>
       <c r="H44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>0.28284271247461906</v>
       </c>
       <c r="I44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>1.8384776310850237</v>
       </c>
       <c r="J44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>0.18384776310850237</v>
       </c>
       <c r="K44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>3.9597979746446663</v>
       </c>
       <c r="L44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>6.0811183182043091</v>
       </c>
       <c r="M44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>1.8384776310850237</v>
       </c>
       <c r="N44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>5.656854249492381E-2</v>
       </c>
       <c r="O44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>0.22627416997969524</v>
       </c>
       <c r="P44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>0.18384776310850237</v>
       </c>
     </row>
@@ -3244,27 +3245,27 @@
         <v>25</v>
       </c>
       <c r="B52">
-        <f t="shared" ref="B52:G52" si="8">(SQRT(B49-1))*B51</f>
+        <f t="shared" ref="B52:G52" si="2">(SQRT(B49-1))*B51</f>
         <v>0.56568542494923812</v>
       </c>
       <c r="C52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>0.84852813742385702</v>
       </c>
       <c r="D52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>0.56568542494923812</v>
       </c>
       <c r="E52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>4.2426406871192854E-2</v>
       </c>
       <c r="F52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>9.8994949366116664E-2</v>
       </c>
       <c r="G52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>7.0710678118654766E-2</v>
       </c>
     </row>
@@ -3647,27 +3648,27 @@
         <v>25</v>
       </c>
       <c r="B80">
-        <f t="shared" ref="B80:G80" si="9">(SQRT(B77-1))*B79</f>
+        <f t="shared" ref="B80:G80" si="3">(SQRT(B77-1))*B79</f>
         <v>5.1429563482495162</v>
       </c>
       <c r="C80">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>5.5425625842204074</v>
       </c>
       <c r="D80">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>3.1304951684997055</v>
       </c>
       <c r="E80">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>5.8889727457341827</v>
       </c>
       <c r="F80">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>9.8386991009990759</v>
       </c>
       <c r="G80">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>10.392304845413264</v>
       </c>
       <c r="I80" s="1"/>
@@ -5447,55 +5448,55 @@
         <v>2.598076211353316</v>
       </c>
       <c r="C206">
-        <f t="shared" ref="C206:O206" si="10">(SQRT(C203-1))*C205</f>
+        <f t="shared" ref="C206:O206" si="4">(SQRT(C203-1))*C205</f>
         <v>0.69282032302755092</v>
       </c>
       <c r="D206">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>2.4248711305964279</v>
       </c>
       <c r="E206">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>0.17320508075688773</v>
       </c>
       <c r="F206">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>0.17320508075688773</v>
       </c>
       <c r="G206">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>0.51961524227066314</v>
       </c>
       <c r="H206">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>1.7320508075688772</v>
       </c>
       <c r="I206">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>0.8660254037844386</v>
       </c>
       <c r="J206">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>0.34641016151377546</v>
       </c>
       <c r="K206">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>0.17320508075688773</v>
       </c>
       <c r="L206">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>2.0784609690826525</v>
       </c>
       <c r="M206">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>1.0392304845413263</v>
       </c>
       <c r="N206">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>0.69282032302755092</v>
       </c>
       <c r="O206">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>0.8660254037844386</v>
       </c>
     </row>
@@ -5861,47 +5862,47 @@
         <v>19.456618411224497</v>
       </c>
       <c r="F215">
-        <f t="shared" ref="F215:P215" si="11">(SQRT(F212-1))*F214</f>
+        <f t="shared" ref="F215:P215" si="5">(SQRT(F212-1))*F214</f>
         <v>11.333137253205752</v>
       </c>
       <c r="G215">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>6.5840716885526085</v>
       </c>
       <c r="H215">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>5.3851648071345036E-2</v>
       </c>
       <c r="I215">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>6.2449979983983987E-2</v>
       </c>
       <c r="J215">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>5.5677643628300216E-2</v>
       </c>
       <c r="K215">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>4.6312417341356733</v>
       </c>
       <c r="L215">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>6.2449979983983987E-2</v>
       </c>
       <c r="M215">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>5.5677643628300216E-2</v>
       </c>
       <c r="N215">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>9.7283092056122484</v>
       </c>
       <c r="O215">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>7.4101282040191458</v>
       </c>
       <c r="P215">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>3.3307656777383787</v>
       </c>
       <c r="Q215">
@@ -6183,71 +6184,71 @@
         <v>4.4858422843430414</v>
       </c>
       <c r="C221">
-        <f t="shared" ref="C221:S221" si="12">(SQRT(C218-1))*C220</f>
+        <f t="shared" ref="C221:S221" si="6">(SQRT(C218-1))*C220</f>
         <v>3.0538040212168167</v>
       </c>
       <c r="D221">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>4.838387231299289</v>
       </c>
       <c r="E221">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>2.8436596139481956</v>
       </c>
       <c r="F221">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>1.6563815985454562</v>
       </c>
       <c r="G221">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>2.943467343117637</v>
       </c>
       <c r="H221">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>5.3851648071345036E-2</v>
       </c>
       <c r="I221">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>6.2449979983983987E-2</v>
       </c>
       <c r="J221">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>5.5677643628300216E-2</v>
       </c>
       <c r="K221">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>2.2402285597679534</v>
       </c>
       <c r="L221">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>0.22481992794234232</v>
       </c>
       <c r="M221">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>0.60131855118564237</v>
       </c>
       <c r="N221">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>3.7416573867739417E-2</v>
       </c>
       <c r="O221">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>4.358898943540674E-2</v>
       </c>
       <c r="P221">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>3.8729833462074169E-2</v>
       </c>
       <c r="Q221">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>0.2731409892344977</v>
       </c>
       <c r="R221">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>4.358898943540674E-2</v>
       </c>
       <c r="S221">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>3.8729833462074169E-2</v>
       </c>
     </row>
@@ -6752,27 +6753,27 @@
         <v>22.074924563804537</v>
       </c>
       <c r="D260">
-        <f t="shared" ref="D260:I260" si="13">(SQRT(D257-1))*D259</f>
+        <f t="shared" ref="D260:I260" si="7">(SQRT(D257-1))*D259</f>
         <v>7.534102157025746</v>
       </c>
       <c r="E260">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>7.3950997288745199</v>
       </c>
       <c r="F260">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>22.602306471077238</v>
       </c>
       <c r="G260">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>19.412136788295612</v>
       </c>
       <c r="H260">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>14.465476141489432</v>
       </c>
       <c r="I260">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>13.311179511974137</v>
       </c>
     </row>
@@ -6955,51 +6956,51 @@
         <v>0</v>
       </c>
       <c r="B267">
-        <f t="shared" ref="B267:M267" si="14">AVERAGE(B265:B266)</f>
+        <f t="shared" ref="B267:M267" si="8">AVERAGE(B265:B266)</f>
         <v>23.265306122448976</v>
       </c>
       <c r="C267">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>2.2448979591836733</v>
       </c>
       <c r="D267">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>10.408163265306122</v>
       </c>
       <c r="E267">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>3.6400000000000019</v>
       </c>
       <c r="F267">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>2.1350000000000007</v>
       </c>
       <c r="G267">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>2.7300000000000013</v>
       </c>
       <c r="H267">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>0.58499999999999885</v>
       </c>
       <c r="I267">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>0.29999999999999938</v>
       </c>
       <c r="J267">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>0.44999999999999907</v>
       </c>
       <c r="K267">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>10.25</v>
       </c>
       <c r="L267">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>15.499999999999998</v>
       </c>
       <c r="M267">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>7.1249999999999982</v>
       </c>
     </row>
@@ -7090,51 +7091,51 @@
         <v>27</v>
       </c>
       <c r="B270">
-        <f t="shared" ref="B270:M270" si="15">AVERAGE(B268:B269)</f>
+        <f t="shared" ref="B270:M270" si="9">AVERAGE(B268:B269)</f>
         <v>3.8775510204081631</v>
       </c>
       <c r="C270">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>0.40816326530612246</v>
       </c>
       <c r="D270">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>5.3061224489795915</v>
       </c>
       <c r="E270">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>0.70000000000000029</v>
       </c>
       <c r="F270">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>0.59500000000000031</v>
       </c>
       <c r="G270">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>0.56000000000000028</v>
       </c>
       <c r="H270">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>0.13499999999999973</v>
       </c>
       <c r="I270">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>0.19499999999999962</v>
       </c>
       <c r="J270">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>0.13499999999999973</v>
       </c>
       <c r="K270">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>0.875</v>
       </c>
       <c r="L270">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1.4999999999999998</v>
       </c>
       <c r="M270">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>0.99999999999999989</v>
       </c>
     </row>
@@ -7143,51 +7144,51 @@
         <v>25</v>
       </c>
       <c r="B271">
-        <f t="shared" ref="B271:M271" si="16">(SQRT(B264-1))*B270</f>
+        <f t="shared" ref="B271:M271" si="10">(SQRT(B264-1))*B270</f>
         <v>5.4836852418548583</v>
       </c>
       <c r="C271">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>0.57723002545840618</v>
       </c>
       <c r="D271">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>7.5039903309592795</v>
       </c>
       <c r="E271">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>0.98994949366116702</v>
       </c>
       <c r="F271">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>0.84145706961199207</v>
       </c>
       <c r="G271">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>0.79195959492893364</v>
       </c>
       <c r="H271">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>0.19091883092036746</v>
       </c>
       <c r="I271">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>0.275771644662753</v>
       </c>
       <c r="J271">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>0.19091883092036746</v>
       </c>
       <c r="K271">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>1.2374368670764582</v>
       </c>
       <c r="L271">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>2.1213203435596424</v>
       </c>
       <c r="M271">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>1.4142135623730949</v>
       </c>
     </row>
@@ -7410,51 +7411,51 @@
         <v>0</v>
       </c>
       <c r="B277">
-        <f t="shared" ref="B277:M277" si="17">AVERAGE(B275:B276)</f>
+        <f t="shared" ref="B277:M277" si="11">AVERAGE(B275:B276)</f>
         <v>12.625</v>
       </c>
       <c r="C277">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>7.625</v>
       </c>
       <c r="D277">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>3.125</v>
       </c>
       <c r="E277">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>9.25</v>
       </c>
       <c r="F277">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>5.75</v>
       </c>
       <c r="G277">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>10.75</v>
       </c>
       <c r="H277">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>0.99000000000000021</v>
       </c>
       <c r="I277">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>1.2600000000000005</v>
       </c>
       <c r="J277">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>1.7100000000000006</v>
       </c>
       <c r="K277">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>10.199999999999999</v>
       </c>
       <c r="L277">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>16.399999999999999</v>
       </c>
       <c r="M277">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>12.4</v>
       </c>
       <c r="Y277" s="12"/>
@@ -7572,51 +7573,51 @@
         <v>27</v>
       </c>
       <c r="B280">
-        <f t="shared" ref="B280:M281" si="18">AVERAGE(B278:B279)</f>
+        <f t="shared" ref="B280:M281" si="12">AVERAGE(B278:B279)</f>
         <v>3.3749999999999996</v>
       </c>
       <c r="C280">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="D280">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>2.5</v>
       </c>
       <c r="E280">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>2.25</v>
       </c>
       <c r="F280">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>1.1249999999999998</v>
       </c>
       <c r="G280">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>2.25</v>
       </c>
       <c r="H280">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>0.33000000000000013</v>
       </c>
       <c r="I280">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>0.36000000000000015</v>
       </c>
       <c r="J280">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>0.42000000000000015</v>
       </c>
       <c r="K280">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>1.6</v>
       </c>
       <c r="L280">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="M280">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>1.8</v>
       </c>
       <c r="Y280" s="12"/>
@@ -7634,51 +7635,51 @@
         <v>25</v>
       </c>
       <c r="B281">
-        <f t="shared" ref="B281:M281" si="19">(SQRT(B274-1))*B280</f>
+        <f t="shared" ref="B281:M281" si="13">(SQRT(B274-1))*B280</f>
         <v>4.7729707730091953</v>
       </c>
       <c r="C281">
-        <f t="shared" si="19"/>
+        <f t="shared" si="13"/>
         <v>4.2426406871192857</v>
       </c>
       <c r="D281">
-        <f t="shared" si="19"/>
+        <f t="shared" si="13"/>
         <v>3.5355339059327378</v>
       </c>
       <c r="E281">
-        <f t="shared" si="19"/>
+        <f t="shared" si="13"/>
         <v>3.1819805153394642</v>
       </c>
       <c r="F281">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>1.3124999999999998</v>
       </c>
       <c r="G281">
-        <f t="shared" si="19"/>
+        <f t="shared" si="13"/>
         <v>3.1819805153394642</v>
       </c>
       <c r="H281">
-        <f t="shared" si="19"/>
+        <f t="shared" si="13"/>
         <v>0.4666904755831216</v>
       </c>
       <c r="I281">
-        <f t="shared" si="19"/>
+        <f t="shared" si="13"/>
         <v>0.50911688245431452</v>
       </c>
       <c r="J281">
-        <f t="shared" si="19"/>
+        <f t="shared" si="13"/>
         <v>0.59396969619670015</v>
       </c>
       <c r="K281">
-        <f t="shared" si="19"/>
+        <f t="shared" si="13"/>
         <v>2.2627416997969525</v>
       </c>
       <c r="L281">
-        <f t="shared" si="19"/>
+        <f t="shared" si="13"/>
         <v>3.1112698372208096</v>
       </c>
       <c r="M281">
-        <f t="shared" si="19"/>
+        <f t="shared" si="13"/>
         <v>2.5455844122715714</v>
       </c>
       <c r="Y281" s="12"/>
@@ -8195,27 +8196,27 @@
         <v>2.7506442902854813</v>
       </c>
       <c r="D301">
-        <f t="shared" ref="D301:I301" si="20">(SQRT(D298-1))*D300</f>
+        <f t="shared" ref="D301:I301" si="14">(SQRT(D298-1))*D300</f>
         <v>0.78589739564398609</v>
       </c>
       <c r="E301">
-        <f t="shared" si="20"/>
+        <f t="shared" si="14"/>
         <v>1.4408136749055085</v>
       </c>
       <c r="F301">
-        <f t="shared" si="20"/>
+        <f t="shared" si="14"/>
         <v>0.52393224481034817</v>
       </c>
       <c r="G301">
-        <f t="shared" si="20"/>
+        <f t="shared" si="14"/>
         <v>0.65491530657195229</v>
       </c>
       <c r="H301">
-        <f t="shared" si="20"/>
+        <f t="shared" si="14"/>
         <v>2.8816273520470852</v>
       </c>
       <c r="I301">
-        <f t="shared" si="20"/>
+        <f t="shared" si="14"/>
         <v>2.7506442902854813</v>
       </c>
       <c r="L301" s="2"/>
@@ -8453,27 +8454,27 @@
         <v>3.0126104138086891</v>
       </c>
       <c r="D307">
-        <f t="shared" ref="D307:I307" si="21">(SQRT(D304-1))*D306</f>
+        <f t="shared" ref="D307:I307" si="15">(SQRT(D304-1))*D306</f>
         <v>0.13098306176160404</v>
       </c>
       <c r="E307">
-        <f t="shared" si="21"/>
+        <f t="shared" si="15"/>
         <v>0.78589836833355642</v>
       </c>
       <c r="F307">
-        <f t="shared" si="21"/>
+        <f t="shared" si="15"/>
         <v>0.13098306176160404</v>
       </c>
       <c r="G307">
-        <f t="shared" si="21"/>
+        <f t="shared" si="15"/>
         <v>4.3224410269525935</v>
       </c>
       <c r="H307">
-        <f t="shared" si="21"/>
+        <f t="shared" si="15"/>
         <v>2.488678166762273</v>
       </c>
       <c r="I307">
-        <f t="shared" si="21"/>
+        <f t="shared" si="15"/>
         <v>3.0126104138086891</v>
       </c>
       <c r="J307" s="2"/>
@@ -8729,47 +8730,47 @@
         <v>4.643274706497559</v>
       </c>
       <c r="C315">
-        <f t="shared" ref="C315:M315" si="22">(SQRT(C312-1))*C314</f>
+        <f t="shared" ref="C315:M315" si="16">(SQRT(C312-1))*C314</f>
         <v>3.9799497484264794</v>
       </c>
       <c r="D315">
-        <f t="shared" si="22"/>
+        <f t="shared" si="16"/>
         <v>4.643274706497559</v>
       </c>
       <c r="E315">
-        <f t="shared" si="22"/>
+        <f t="shared" si="16"/>
         <v>3.3166247903553998</v>
       </c>
       <c r="F315">
-        <f t="shared" si="22"/>
+        <f t="shared" si="16"/>
         <v>3.9799497484264794</v>
       </c>
       <c r="G315">
-        <f t="shared" si="22"/>
+        <f t="shared" si="16"/>
         <v>4.643274706497559</v>
       </c>
       <c r="H315">
-        <f t="shared" si="22"/>
+        <f t="shared" si="16"/>
         <v>1.3266499161421601</v>
       </c>
       <c r="I315">
-        <f t="shared" si="22"/>
+        <f t="shared" si="16"/>
         <v>1.9899748742132397</v>
       </c>
       <c r="J315">
-        <f t="shared" si="22"/>
+        <f t="shared" si="16"/>
         <v>1.3266499161421601</v>
       </c>
       <c r="K315">
-        <f t="shared" si="22"/>
+        <f t="shared" si="16"/>
         <v>0.33166247903554003</v>
       </c>
       <c r="L315">
-        <f t="shared" si="22"/>
+        <f t="shared" si="16"/>
         <v>0.66332495807108005</v>
       </c>
       <c r="M315">
-        <f t="shared" si="22"/>
+        <f t="shared" si="16"/>
         <v>0.66332495807108005</v>
       </c>
     </row>
@@ -8954,47 +8955,47 @@
         <v>2.6532998322843202</v>
       </c>
       <c r="C322">
-        <f t="shared" ref="C322:M322" si="23">(SQRT(C319-1))*C321</f>
+        <f t="shared" ref="C322:M322" si="17">(SQRT(C319-1))*C321</f>
         <v>1.9899748742132397</v>
       </c>
       <c r="D322">
-        <f t="shared" si="23"/>
+        <f t="shared" si="17"/>
         <v>1.3266499161421601</v>
       </c>
       <c r="E322">
-        <f t="shared" si="23"/>
+        <f t="shared" si="17"/>
         <v>0.33166247903554003</v>
       </c>
       <c r="F322">
-        <f t="shared" si="23"/>
+        <f t="shared" si="17"/>
         <v>0.33166247903554003</v>
       </c>
       <c r="G322">
-        <f t="shared" si="23"/>
+        <f t="shared" si="17"/>
         <v>0.33166247903554003</v>
       </c>
       <c r="H322">
-        <f t="shared" si="23"/>
+        <f t="shared" si="17"/>
         <v>2.3216373532487795</v>
       </c>
       <c r="I322">
-        <f t="shared" si="23"/>
+        <f t="shared" si="17"/>
         <v>1.3266499161421601</v>
       </c>
       <c r="J322">
-        <f t="shared" si="23"/>
+        <f t="shared" si="17"/>
         <v>0.99498743710661985</v>
       </c>
       <c r="K322">
-        <f t="shared" si="23"/>
+        <f t="shared" si="17"/>
         <v>3.3166247903553998E-2</v>
       </c>
       <c r="L322">
-        <f t="shared" si="23"/>
+        <f t="shared" si="17"/>
         <v>3.3166247903553998E-2</v>
       </c>
       <c r="M322">
-        <f t="shared" si="23"/>
+        <f t="shared" si="17"/>
         <v>3.3166247903553998E-2</v>
       </c>
     </row>
@@ -9067,7 +9068,7 @@
         <v>0.2449489742783178</v>
       </c>
       <c r="C329">
-        <f t="shared" ref="C329" si="24">(SQRT(C326-1))*C328</f>
+        <f t="shared" ref="C329" si="18">(SQRT(C326-1))*C328</f>
         <v>2.4494897427831779</v>
       </c>
     </row>
@@ -9132,7 +9133,7 @@
         <v>1.2247448713915889</v>
       </c>
       <c r="C336">
-        <f t="shared" ref="C336" si="25">(SQRT(C333-1))*C335</f>
+        <f t="shared" ref="C336" si="19">(SQRT(C333-1))*C335</f>
         <v>19.595917942265423</v>
       </c>
     </row>
@@ -9445,27 +9446,27 @@
         <v>25</v>
       </c>
       <c r="B358">
-        <f t="shared" ref="B358:G358" si="26">(SQRT(B355-1))*B357</f>
+        <f t="shared" ref="B358:G358" si="20">(SQRT(B355-1))*B357</f>
         <v>3.5355339059327378</v>
       </c>
       <c r="C358">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>2.8284271247461903</v>
       </c>
       <c r="D358">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>0.70710678118654757</v>
       </c>
       <c r="E358">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="F358">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>0.70710678118654757</v>
       </c>
       <c r="G358">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>0.42426406871192851</v>
       </c>
     </row>
@@ -9649,11 +9650,11 @@
         <v>10.748023074035522</v>
       </c>
       <c r="D372">
-        <f t="shared" ref="D372:E372" si="27">(SQRT(D369-1))*D371</f>
+        <f t="shared" ref="D372:E372" si="21">(SQRT(D369-1))*D371</f>
         <v>12.303657992645928</v>
       </c>
       <c r="E372">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>6.2225396744416193</v>
       </c>
       <c r="J372" s="2"/>
@@ -9748,15 +9749,15 @@
         <v>0</v>
       </c>
       <c r="B380" s="3">
-        <f t="shared" ref="B380:D380" si="28">AVERAGE(B377:B379)</f>
+        <f t="shared" ref="B380:D380" si="22">AVERAGE(B377:B379)</f>
         <v>3.72</v>
       </c>
       <c r="C380" s="3">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>4.376666666666666</v>
       </c>
       <c r="D380" s="3">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>5.9866666666666672</v>
       </c>
     </row>
@@ -9807,15 +9808,15 @@
         <v>27</v>
       </c>
       <c r="B384" s="3">
-        <f t="shared" ref="B384:D384" si="29">AVERAGE(B381:B383)</f>
+        <f t="shared" ref="B384:D384" si="23">AVERAGE(B381:B383)</f>
         <v>0.89666666666666661</v>
       </c>
       <c r="C384" s="3">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>1.3566666666666667</v>
       </c>
       <c r="D384" s="3">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>1.1333333333333335</v>
       </c>
     </row>
@@ -9824,15 +9825,15 @@
         <v>25</v>
       </c>
       <c r="B385" s="6">
-        <f t="shared" ref="B385:D385" si="30">(SQRT(B376-1))*B384</f>
+        <f t="shared" ref="B385:D385" si="24">(SQRT(B376-1))*B384</f>
         <v>1.2680781609278753</v>
       </c>
       <c r="C385" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="24"/>
         <v>1.9186163996194991</v>
       </c>
       <c r="D385" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="24"/>
         <v>1.602775370689508</v>
       </c>
     </row>
@@ -9913,15 +9914,15 @@
         <v>0</v>
       </c>
       <c r="B391" s="3">
-        <f t="shared" ref="B391:D391" si="31">AVERAGE(B388:B390)</f>
+        <f t="shared" ref="B391:D391" si="25">AVERAGE(B388:B390)</f>
         <v>0.25333333333333335</v>
       </c>
       <c r="C391" s="3">
-        <f t="shared" si="31"/>
+        <f t="shared" si="25"/>
         <v>0.37666666666666665</v>
       </c>
       <c r="D391" s="3">
-        <f t="shared" si="31"/>
+        <f t="shared" si="25"/>
         <v>0.46333333333333337</v>
       </c>
       <c r="E391" s="2"/>
@@ -9974,15 +9975,15 @@
         <v>27</v>
       </c>
       <c r="B395" s="3">
-        <f t="shared" ref="B395:D395" si="32">AVERAGE(B392:B394)</f>
+        <f t="shared" ref="B395:D395" si="26">AVERAGE(B392:B394)</f>
         <v>0.10333333333333333</v>
       </c>
       <c r="C395" s="3">
-        <f t="shared" si="32"/>
+        <f t="shared" si="26"/>
         <v>0.22333333333333336</v>
       </c>
       <c r="D395" s="3">
-        <f t="shared" si="32"/>
+        <f t="shared" si="26"/>
         <v>0.18666666666666668</v>
       </c>
       <c r="I395" s="1"/>
@@ -9992,15 +9993,15 @@
         <v>25</v>
       </c>
       <c r="B396" s="6">
-        <f t="shared" ref="B396:D396" si="33">(SQRT(B387-1))*B395</f>
+        <f t="shared" ref="B396:D396" si="27">(SQRT(B387-1))*B395</f>
         <v>0.14613540144521983</v>
       </c>
       <c r="C396" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="27"/>
         <v>0.31584102892999127</v>
       </c>
       <c r="D396" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="27"/>
         <v>0.26398653164297775</v>
       </c>
     </row>
@@ -10044,7 +10045,7 @@
       <c r="A400" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B400" s="3">
+      <c r="B400" s="22">
         <v>1.367</v>
       </c>
       <c r="C400" s="6">
@@ -10059,7 +10060,7 @@
       <c r="A401" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B401" s="3">
+      <c r="B401" s="22">
         <v>0.36599999999999999</v>
       </c>
       <c r="C401" s="6">
@@ -10083,7 +10084,7 @@
         <v>2.0264577469071492</v>
       </c>
       <c r="D402">
-        <f t="shared" ref="D402" si="34">(SQRT(D399-1))*D401</f>
+        <f t="shared" ref="D402" si="28">(SQRT(D399-1))*D401</f>
         <v>2.0762071187624804</v>
       </c>
     </row>
@@ -10119,7 +10120,7 @@
       <c r="A405" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B405" s="3">
+      <c r="B405" s="22">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="C405" s="6">
@@ -10133,7 +10134,7 @@
       <c r="A406" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B406" s="3">
+      <c r="B406" s="22">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="C406" s="6">
@@ -10156,7 +10157,7 @@
         <v>0.13929824119492681</v>
       </c>
       <c r="D407">
-        <f t="shared" ref="D407" si="35">(SQRT(D404-1))*D406</f>
+        <f t="shared" ref="D407" si="29">(SQRT(D404-1))*D406</f>
         <v>0.16914786430812537</v>
       </c>
     </row>
@@ -10231,7 +10232,7 @@
       <c r="D412" s="2">
         <v>11.6</v>
       </c>
-      <c r="E412" s="3">
+      <c r="E412" s="22">
         <v>3.3</v>
       </c>
       <c r="F412" s="6">
@@ -10254,7 +10255,7 @@
       <c r="D413" s="2">
         <v>0.2</v>
       </c>
-      <c r="E413" s="3">
+      <c r="E413" s="22">
         <v>0.2</v>
       </c>
       <c r="F413" s="6">
@@ -10277,7 +10278,7 @@
         <v>0.28284271247461906</v>
       </c>
       <c r="D414">
-        <f t="shared" ref="D414" si="36">(SQRT(D411-1))*D413</f>
+        <f t="shared" ref="D414" si="30">(SQRT(D411-1))*D413</f>
         <v>0.28284271247461906</v>
       </c>
       <c r="E414">
@@ -10289,7 +10290,7 @@
         <v>0.28284271247461906</v>
       </c>
       <c r="G414">
-        <f t="shared" ref="G414" si="37">(SQRT(G411-1))*G413</f>
+        <f t="shared" ref="G414" si="31">(SQRT(G411-1))*G413</f>
         <v>0.56568542494923812</v>
       </c>
       <c r="H414" s="6"/>
@@ -10334,7 +10335,7 @@
       <c r="A417" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B417" s="3">
+      <c r="B417" s="22">
         <v>17</v>
       </c>
       <c r="C417" s="6">
@@ -10349,7 +10350,7 @@
       <c r="A418" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B418" s="3">
+      <c r="B418" s="22">
         <v>1</v>
       </c>
       <c r="C418" s="6">
@@ -10372,7 +10373,7 @@
         <v>8.4852813742385713</v>
       </c>
       <c r="D419">
-        <f t="shared" ref="D419" si="38">(SQRT(D416-1))*D418</f>
+        <f t="shared" ref="D419" si="32">(SQRT(D416-1))*D418</f>
         <v>9.8994949366116654</v>
       </c>
     </row>
@@ -10432,7 +10433,7 @@
       <c r="A423" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B423" s="3">
+      <c r="B423" s="22">
         <v>3.5</v>
       </c>
       <c r="C423" s="6">
@@ -10441,7 +10442,7 @@
       <c r="D423" s="2">
         <v>5.7</v>
       </c>
-      <c r="E423" s="3">
+      <c r="E423" s="22">
         <v>1.6</v>
       </c>
       <c r="F423" s="6">
@@ -10455,7 +10456,7 @@
       <c r="A424" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B424" s="3">
+      <c r="B424" s="22">
         <v>0.2</v>
       </c>
       <c r="C424" s="6">
@@ -10464,7 +10465,7 @@
       <c r="D424" s="2">
         <v>0.3</v>
       </c>
-      <c r="E424" s="3">
+      <c r="E424" s="22">
         <v>0.2</v>
       </c>
       <c r="F424" s="6">
@@ -10487,7 +10488,7 @@
         <v>0.28284271247461906</v>
       </c>
       <c r="D425">
-        <f t="shared" ref="D425" si="39">(SQRT(D422-1))*D424</f>
+        <f t="shared" ref="D425" si="33">(SQRT(D422-1))*D424</f>
         <v>0.42426406871192851</v>
       </c>
       <c r="E425">
@@ -10499,7 +10500,7 @@
         <v>0.28284271247461906</v>
       </c>
       <c r="G425">
-        <f t="shared" ref="G425" si="40">(SQRT(G422-1))*G424</f>
+        <f t="shared" ref="G425" si="34">(SQRT(G422-1))*G424</f>
         <v>0.42426406871192851</v>
       </c>
     </row>
@@ -10537,7 +10538,7 @@
       <c r="A428" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B428" s="3">
+      <c r="B428" s="22">
         <v>21</v>
       </c>
       <c r="C428" s="6">
@@ -10551,7 +10552,7 @@
       <c r="A429" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B429" s="3">
+      <c r="B429" s="22">
         <v>2</v>
       </c>
       <c r="C429" s="6">
@@ -10574,7 +10575,7 @@
         <v>2.8284271247461903</v>
       </c>
       <c r="D430">
-        <f t="shared" ref="D430" si="41">(SQRT(D427-1))*D429</f>
+        <f t="shared" ref="D430" si="35">(SQRT(D427-1))*D429</f>
         <v>2.8284271247461903</v>
       </c>
     </row>
@@ -10602,7 +10603,7 @@
       <c r="A433" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B433">
+      <c r="B433" s="19">
         <v>5</v>
       </c>
       <c r="C433">
@@ -10613,7 +10614,7 @@
       <c r="A434" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B434" s="3">
+      <c r="B434" s="22">
         <v>26.1</v>
       </c>
       <c r="C434" s="2">
@@ -10624,7 +10625,7 @@
       <c r="A435" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B435" s="3">
+      <c r="B435" s="22">
         <v>1.2</v>
       </c>
       <c r="C435" s="2">
@@ -10640,7 +10641,7 @@
         <v>2.4</v>
       </c>
       <c r="C436">
-        <f t="shared" ref="C436" si="42">(SQRT(C433-1))*C435</f>
+        <f t="shared" ref="C436" si="36">(SQRT(C433-1))*C435</f>
         <v>2</v>
       </c>
       <c r="E436" s="6"/>
@@ -10671,7 +10672,7 @@
       <c r="A439" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B439" s="3">
+      <c r="B439" s="22">
         <v>9</v>
       </c>
       <c r="C439" s="2">
@@ -10682,7 +10683,7 @@
       <c r="A440" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B440" s="3">
+      <c r="B440" s="22">
         <v>1</v>
       </c>
       <c r="C440" s="2">
@@ -10698,7 +10699,7 @@
         <v>2</v>
       </c>
       <c r="C441">
-        <f t="shared" ref="C441" si="43">(SQRT(C438-1))*C440</f>
+        <f t="shared" ref="C441" si="37">(SQRT(C438-1))*C440</f>
         <v>2</v>
       </c>
     </row>
@@ -10815,23 +10816,23 @@
         <v>0</v>
       </c>
       <c r="C447">
-        <f t="shared" ref="C447:E447" si="44">(SQRT(C444-1))*C446</f>
+        <f t="shared" ref="C447:E447" si="38">(SQRT(C444-1))*C446</f>
         <v>0</v>
       </c>
       <c r="D447">
-        <f t="shared" si="44"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="E447">
-        <f t="shared" si="44"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="F447">
-        <f t="shared" ref="F447:G447" si="45">(SQRT(F444-1))*F446</f>
+        <f t="shared" ref="F447:G447" si="39">(SQRT(F444-1))*F446</f>
         <v>0</v>
       </c>
       <c r="G447">
-        <f t="shared" si="45"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
     </row>
@@ -10912,15 +10913,15 @@
         <v>0</v>
       </c>
       <c r="C452">
-        <f t="shared" ref="C452:E452" si="46">(SQRT(C449-1))*C451</f>
+        <f t="shared" ref="C452:E452" si="40">(SQRT(C449-1))*C451</f>
         <v>0</v>
       </c>
       <c r="D452">
-        <f t="shared" si="46"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="E452">
-        <f t="shared" si="46"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
@@ -11005,11 +11006,11 @@
         <v>1.4142135623730951</v>
       </c>
       <c r="C458">
-        <f t="shared" ref="C458:D458" si="47">(SQRT(C455-1))*C457</f>
+        <f t="shared" ref="C458:D458" si="41">(SQRT(C455-1))*C457</f>
         <v>0.70710678118654757</v>
       </c>
       <c r="D458">
-        <f t="shared" si="47"/>
+        <f t="shared" si="41"/>
         <v>7.0710678118654755</v>
       </c>
       <c r="E458" s="1"/>
@@ -11102,13 +11103,13 @@
       <c r="A463" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B463" s="3">
+      <c r="B463" s="22">
         <v>19.7</v>
       </c>
       <c r="C463" s="2">
         <v>15.6</v>
       </c>
-      <c r="D463" s="3">
+      <c r="D463" s="22">
         <v>0.1</v>
       </c>
       <c r="E463" s="2">
@@ -11127,13 +11128,13 @@
       <c r="A464" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B464" s="3">
+      <c r="B464" s="22">
         <v>2.6</v>
       </c>
       <c r="C464" s="2">
         <v>2.5</v>
       </c>
-      <c r="D464" s="3">
+      <c r="D464" s="22">
         <v>0.1</v>
       </c>
       <c r="E464" s="2">
@@ -11149,7 +11150,7 @@
         <v>7.8000000000000007</v>
       </c>
       <c r="C465">
-        <f t="shared" ref="C465:E465" si="48">(SQRT(C462-1))*C464</f>
+        <f t="shared" ref="C465:E465" si="42">(SQRT(C462-1))*C464</f>
         <v>7.5</v>
       </c>
       <c r="D465">
@@ -11157,7 +11158,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="E465">
-        <f t="shared" si="48"/>
+        <f t="shared" si="42"/>
         <v>0.30000000000000004</v>
       </c>
     </row>
@@ -11192,7 +11193,7 @@
       <c r="A469" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B469" s="3">
+      <c r="B469" s="22">
         <v>23.6</v>
       </c>
       <c r="C469" s="2">
@@ -11203,7 +11204,7 @@
       <c r="A470" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B470" s="3">
+      <c r="B470" s="22">
         <v>4.0999999999999996</v>
       </c>
       <c r="C470" s="2">
@@ -11219,7 +11220,7 @@
         <v>9.1678787077491375</v>
       </c>
       <c r="C471">
-        <f t="shared" ref="C471" si="49">(SQRT(C468-1))*C470</f>
+        <f t="shared" ref="C471" si="43">(SQRT(C468-1))*C470</f>
         <v>11.403946685248927</v>
       </c>
     </row>
@@ -11254,7 +11255,7 @@
       <c r="A475" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B475" s="3">
+      <c r="B475" s="22">
         <v>17.600000000000001</v>
       </c>
       <c r="C475" s="2">
@@ -11265,7 +11266,7 @@
       <c r="A476" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B476" s="3">
+      <c r="B476" s="22">
         <v>2.4</v>
       </c>
       <c r="C476" s="2">
@@ -11281,7 +11282,7 @@
         <v>4.1569219381653051</v>
       </c>
       <c r="C477">
-        <f t="shared" ref="C477" si="50">(SQRT(C474-1))*C476</f>
+        <f t="shared" ref="C477" si="44">(SQRT(C474-1))*C476</f>
         <v>11.085125168440815</v>
       </c>
     </row>
@@ -11316,7 +11317,7 @@
       <c r="A481" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B481" s="3">
+      <c r="B481" s="22">
         <v>44.1</v>
       </c>
       <c r="C481" s="2">
@@ -11327,7 +11328,7 @@
       <c r="A482" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B482" s="3">
+      <c r="B482" s="22">
         <v>11.6</v>
       </c>
       <c r="C482" s="2">
@@ -11343,7 +11344,7 @@
         <v>20.091789367798974</v>
       </c>
       <c r="C483">
-        <f t="shared" ref="C483" si="51">(SQRT(C480-1))*C482</f>
+        <f t="shared" ref="C483" si="45">(SQRT(C480-1))*C482</f>
         <v>12.124355652982141</v>
       </c>
     </row>
@@ -11378,7 +11379,7 @@
       <c r="A487" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B487" s="3">
+      <c r="B487" s="22">
         <v>1.5</v>
       </c>
       <c r="C487" s="2">
@@ -11389,7 +11390,7 @@
       <c r="A488" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B488" s="3">
+      <c r="B488" s="22">
         <v>0.3</v>
       </c>
       <c r="C488" s="2">
@@ -11405,7 +11406,7 @@
         <v>0.89999999999999991</v>
       </c>
       <c r="C489">
-        <f t="shared" ref="C489" si="52">(SQRT(C486-1))*C488</f>
+        <f t="shared" ref="C489" si="46">(SQRT(C486-1))*C488</f>
         <v>0.89999999999999991</v>
       </c>
     </row>
@@ -11440,7 +11441,7 @@
       <c r="A493" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B493" s="3">
+      <c r="B493" s="22">
         <v>1</v>
       </c>
       <c r="C493" s="2">
@@ -11451,7 +11452,7 @@
       <c r="A494" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B494" s="3">
+      <c r="B494" s="22">
         <v>0.4</v>
       </c>
       <c r="C494" s="2">
@@ -11467,7 +11468,7 @@
         <v>0.89442719099991597</v>
       </c>
       <c r="C495">
-        <f t="shared" ref="C495" si="53">(SQRT(C492-1))*C494</f>
+        <f t="shared" ref="C495" si="47">(SQRT(C492-1))*C494</f>
         <v>1.7888543819998319</v>
       </c>
     </row>
@@ -11502,7 +11503,7 @@
       <c r="A499" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B499" s="3">
+      <c r="B499" s="22">
         <v>0.2</v>
       </c>
       <c r="C499" s="2">
@@ -11513,7 +11514,7 @@
       <c r="A500" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B500" s="3">
+      <c r="B500" s="22">
         <v>0.2</v>
       </c>
       <c r="C500" s="2">
@@ -11529,7 +11530,7 @@
         <v>0.34641016151377546</v>
       </c>
       <c r="C501">
-        <f t="shared" ref="C501" si="54">(SQRT(C498-1))*C500</f>
+        <f t="shared" ref="C501" si="48">(SQRT(C498-1))*C500</f>
         <v>0.51961524227066314</v>
       </c>
     </row>
@@ -11655,52 +11656,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="Control 1">
-          <controlPr defaultSize="0" autoPict="0" r:id="rId5">
+        <control shapeId="1026" r:id="rId4" name="Control 2">
+          <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>76200</xdr:colOff>
-                <xdr:row>95</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
+                <xdr:colOff>66675</xdr:colOff>
+                <xdr:row>97</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>295275</xdr:colOff>
-                <xdr:row>97</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:colOff>219075</xdr:colOff>
+                <xdr:row>98</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="Control 1"/>
+        <control shapeId="1026" r:id="rId4" name="Control 2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId6" name="Control 2">
-          <controlPr defaultSize="0" autoPict="0" r:id="rId5">
+        <control shapeId="1025" r:id="rId6" name="Control 1">
+          <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>76200</xdr:colOff>
-                <xdr:row>95</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
+                <xdr:colOff>66675</xdr:colOff>
+                <xdr:row>97</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>295275</xdr:colOff>
-                <xdr:row>97</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:colOff>219075</xdr:colOff>
+                <xdr:row>98</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId6" name="Control 2"/>
+        <control shapeId="1025" r:id="rId6" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Fixed error on Fule+Covington+etal-2002
This paper was excluded, but I accidentally had it checked as "Yes" on
UsedOrNot. I fixed the error by taking it out of papers-used-only.csv
and switching it to "No" in papers.csv.
</commit_message>
<xml_diff>
--- a/Data Extraction Workbook/Copy of Excel Calculator for Means of means and SE's ONLY USED PAPERS.xlsx
+++ b/Data Extraction Workbook/Copy of Excel Calculator for Means of means and SE's ONLY USED PAPERS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="119">
   <si>
     <t>mean</t>
   </si>
@@ -368,6 +368,12 @@
   <si>
     <t>Shive+Sieg</t>
   </si>
+  <si>
+    <t>This was Canopy Cover</t>
+  </si>
+  <si>
+    <t>This is the correct data</t>
+  </si>
 </sst>
 </file>
 
@@ -532,15 +538,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>54429</xdr:colOff>
-          <xdr:row>99</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:colOff>40821</xdr:colOff>
+          <xdr:row>102</xdr:row>
+          <xdr:rowOff>13607</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>273504</xdr:colOff>
-          <xdr:row>100</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:colOff>193221</xdr:colOff>
+          <xdr:row>102</xdr:row>
+          <xdr:rowOff>175532</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -573,15 +579,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>54429</xdr:colOff>
-          <xdr:row>99</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:colOff>40821</xdr:colOff>
+          <xdr:row>102</xdr:row>
+          <xdr:rowOff>13607</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>273504</xdr:colOff>
-          <xdr:row>100</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:colOff>193221</xdr:colOff>
+          <xdr:row>102</xdr:row>
+          <xdr:rowOff>175532</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -902,8 +908,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AR539"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A231" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A262" sqref="A262"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J100" sqref="J100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3899,113 +3905,154 @@
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A97" s="13" t="s">
+      <c r="A97" s="24" t="s">
         <v>51</v>
       </c>
+      <c r="B97" t="s">
+        <v>117</v>
+      </c>
+      <c r="C97" s="11"/>
+      <c r="D97" s="11"/>
+      <c r="F97" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="9" t="s">
+      <c r="A98" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E98" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F98" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G98" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H98" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A99" s="10" t="s">
+      <c r="A99" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B99">
+      <c r="B99" s="11">
         <v>20</v>
       </c>
-      <c r="C99">
+      <c r="C99" s="11">
         <v>20</v>
       </c>
-      <c r="D99">
+      <c r="D99" s="11">
         <v>20</v>
       </c>
+      <c r="F99" s="6">
+        <v>20</v>
+      </c>
+      <c r="G99" s="6">
+        <v>20</v>
+      </c>
+      <c r="H99" s="6">
+        <v>20</v>
+      </c>
     </row>
     <row r="100" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A100" s="10" t="s">
+      <c r="A100" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B100">
+      <c r="B100" s="11">
         <v>52.3</v>
       </c>
-      <c r="C100">
+      <c r="C100" s="11">
         <v>37.6</v>
       </c>
-      <c r="D100">
+      <c r="D100" s="11">
         <v>53.7</v>
       </c>
+      <c r="F100" s="6"/>
+      <c r="G100" s="6"/>
+      <c r="H100" s="6"/>
     </row>
     <row r="101" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A101" s="10" t="s">
+      <c r="A101" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B101">
+      <c r="B101" s="11">
         <v>4.2</v>
       </c>
-      <c r="C101">
+      <c r="C101" s="11">
         <v>2.8</v>
       </c>
-      <c r="D101">
+      <c r="D101" s="11">
         <v>4.4000000000000004</v>
       </c>
+      <c r="F101" s="6"/>
+      <c r="G101" s="6"/>
+      <c r="H101" s="6"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A102" s="9" t="s">
+      <c r="A102" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B102">
+      <c r="B102" s="11">
         <f>(SQRT(B99-1))*B101</f>
         <v>18.307375562870831</v>
       </c>
-      <c r="C102">
+      <c r="C102" s="11">
         <f>(SQRT(C99-1))*C101</f>
         <v>12.204917041913886</v>
       </c>
-      <c r="D102">
+      <c r="D102" s="11">
         <f>(SQRT(D99-1))*D101</f>
         <v>19.179155351578967</v>
       </c>
+      <c r="F102" s="6"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="8" t="s">
+      <c r="A103" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C103">
+      <c r="B103" s="11"/>
+      <c r="C103" s="11">
         <v>-1.2418</v>
       </c>
-      <c r="D103">
+      <c r="D103" s="11">
         <v>9.8100000000000007E-2</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="8" t="s">
+      <c r="A104" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C104">
+      <c r="B104" s="11"/>
+      <c r="C104" s="11">
         <v>-2.1156000000000001</v>
       </c>
-      <c r="D104">
+      <c r="D104" s="11">
         <v>-0.70250000000000001</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="8" t="s">
+      <c r="A105" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C105">
+      <c r="B105" s="11"/>
+      <c r="C105" s="11">
         <v>-0.3679</v>
       </c>
-      <c r="D105">
+      <c r="D105" s="11">
         <v>0.89880000000000004</v>
       </c>
     </row>
@@ -11701,52 +11748,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="Control 1">
-          <controlPr defaultSize="0" autoPict="0" r:id="rId5">
+        <control shapeId="1026" r:id="rId4" name="Control 2">
+          <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>47625</xdr:colOff>
-                <xdr:row>100</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>102</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>266700</xdr:colOff>
-                <xdr:row>101</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
+                <xdr:colOff>190500</xdr:colOff>
+                <xdr:row>102</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="Control 1"/>
+        <control shapeId="1026" r:id="rId4" name="Control 2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId6" name="Control 2">
-          <controlPr defaultSize="0" autoPict="0" r:id="rId5">
+        <control shapeId="1025" r:id="rId6" name="Control 1">
+          <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>47625</xdr:colOff>
-                <xdr:row>100</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>102</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>266700</xdr:colOff>
-                <xdr:row>101</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
+                <xdr:colOff>190500</xdr:colOff>
+                <xdr:row>102</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId6" name="Control 2"/>
+        <control shapeId="1025" r:id="rId6" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Fixed some errors in response-vars, cleaned papers-used-only.csv
I found errors in my data extraction from 2 papers and fixed the issues.
I also put two papers that were out of order into order in
papers-used-only.csv.
</commit_message>
<xml_diff>
--- a/Data Extraction Workbook/Copy of Excel Calculator for Means of means and SE's ONLY USED PAPERS.xlsx
+++ b/Data Extraction Workbook/Copy of Excel Calculator for Means of means and SE's ONLY USED PAPERS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="119">
   <si>
     <t>mean</t>
   </si>
@@ -481,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -509,6 +509,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,15 +539,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>40821</xdr:colOff>
+          <xdr:colOff>35379</xdr:colOff>
           <xdr:row>102</xdr:row>
-          <xdr:rowOff>13607</xdr:rowOff>
+          <xdr:rowOff>10886</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>193221</xdr:colOff>
-          <xdr:row>102</xdr:row>
-          <xdr:rowOff>175532</xdr:rowOff>
+          <xdr:colOff>254454</xdr:colOff>
+          <xdr:row>103</xdr:row>
+          <xdr:rowOff>54429</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -579,15 +580,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>40821</xdr:colOff>
+          <xdr:colOff>35379</xdr:colOff>
           <xdr:row>102</xdr:row>
-          <xdr:rowOff>13607</xdr:rowOff>
+          <xdr:rowOff>10886</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>193221</xdr:colOff>
-          <xdr:row>102</xdr:row>
-          <xdr:rowOff>175532</xdr:rowOff>
+          <xdr:colOff>254454</xdr:colOff>
+          <xdr:row>103</xdr:row>
+          <xdr:rowOff>54429</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -908,8 +909,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AR539"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J100" sqref="J100"/>
+    <sheetView tabSelected="1" topLeftCell="A159" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A188" sqref="A188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6709,12 +6710,6 @@
       <c r="A255" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E255" t="s">
-        <v>14</v>
-      </c>
-      <c r="F255" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="256" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A256" s="4" t="s">
@@ -6729,11 +6724,11 @@
       <c r="D256" t="s">
         <v>13</v>
       </c>
-      <c r="E256">
-        <v>36</v>
-      </c>
-      <c r="F256">
-        <v>94</v>
+      <c r="E256" t="s">
+        <v>14</v>
+      </c>
+      <c r="F256" t="s">
+        <v>10</v>
       </c>
       <c r="G256" t="s">
         <v>11</v>
@@ -6759,10 +6754,10 @@
         <v>94</v>
       </c>
       <c r="E257">
-        <v>-0.15625</v>
+        <v>36</v>
       </c>
       <c r="F257">
-        <v>1.4062499999999998</v>
+        <v>94</v>
       </c>
       <c r="G257">
         <v>36</v>
@@ -6788,10 +6783,10 @@
         <v>-0.15625</v>
       </c>
       <c r="E258">
-        <v>1.25</v>
+        <v>-0.15625</v>
       </c>
       <c r="F258">
-        <v>2.34375</v>
+        <v>1.4062499999999998</v>
       </c>
       <c r="G258">
         <v>3.75</v>
@@ -6817,12 +6812,10 @@
         <v>0.78125</v>
       </c>
       <c r="E259">
-        <f t="shared" ref="D259:I260" si="13">(SQRT(E256-1))*E258</f>
-        <v>7.3950997288745199</v>
+        <v>1.25</v>
       </c>
       <c r="F259">
-        <f t="shared" si="13"/>
-        <v>22.602306471077238</v>
+        <v>2.34375</v>
       </c>
       <c r="G259">
         <v>3.2812499999999996</v>
@@ -6847,8 +6840,16 @@
         <v>22.074924563804537</v>
       </c>
       <c r="D260">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="D259:I260" si="13">(SQRT(D257-1))*D259</f>
         <v>7.534102157025746</v>
+      </c>
+      <c r="E260">
+        <f>(SQRT(E257-1))*E259</f>
+        <v>7.3950997288745199</v>
+      </c>
+      <c r="F260">
+        <f>(SQRT(F257-1))*F259</f>
+        <v>22.602306471077238</v>
       </c>
       <c r="G260">
         <f t="shared" si="13"/>
@@ -6872,12 +6873,6 @@
       <c r="A262" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="E262" t="s">
-        <v>89</v>
-      </c>
-      <c r="F262" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="263" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A263" s="9" t="s">
@@ -6892,11 +6887,11 @@
       <c r="D263" t="s">
         <v>3</v>
       </c>
-      <c r="E263">
-        <v>3</v>
-      </c>
-      <c r="F263">
-        <v>3</v>
+      <c r="E263" t="s">
+        <v>89</v>
+      </c>
+      <c r="F263" t="s">
+        <v>14</v>
       </c>
       <c r="G263" t="s">
         <v>15</v>
@@ -6934,10 +6929,10 @@
         <v>3</v>
       </c>
       <c r="E264">
-        <v>3.5000000000000018</v>
+        <v>3</v>
       </c>
       <c r="F264">
-        <v>2.3100000000000009</v>
+        <v>3</v>
       </c>
       <c r="G264">
         <v>3</v>
@@ -6975,10 +6970,10 @@
         <v>11.428571428571427</v>
       </c>
       <c r="E265">
-        <v>3.780000000000002</v>
+        <v>3.5000000000000018</v>
       </c>
       <c r="F265">
-        <v>1.9600000000000009</v>
+        <v>2.3100000000000009</v>
       </c>
       <c r="G265">
         <v>2.100000000000001</v>
@@ -7016,12 +7011,10 @@
         <v>9.3877551020408152</v>
       </c>
       <c r="E266">
-        <f t="shared" ref="B266:M267" si="14">AVERAGE(E264:E265)</f>
-        <v>3.6400000000000019</v>
+        <v>3.780000000000002</v>
       </c>
       <c r="F266">
-        <f t="shared" si="14"/>
-        <v>2.1350000000000007</v>
+        <v>1.9600000000000009</v>
       </c>
       <c r="G266">
         <v>3.3600000000000012</v>
@@ -7050,7 +7043,7 @@
         <v>0</v>
       </c>
       <c r="B267">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="B266:M267" si="14">AVERAGE(B265:B266)</f>
         <v>23.265306122448976</v>
       </c>
       <c r="C267">
@@ -7062,10 +7055,12 @@
         <v>10.408163265306122</v>
       </c>
       <c r="E267">
-        <v>0.70000000000000029</v>
+        <f>AVERAGE(E265:E266)</f>
+        <v>3.6400000000000019</v>
       </c>
       <c r="F267">
-        <v>0.63000000000000034</v>
+        <f>AVERAGE(F265:F266)</f>
+        <v>2.1350000000000007</v>
       </c>
       <c r="G267">
         <f t="shared" si="14"/>
@@ -7113,7 +7108,7 @@
         <v>0.70000000000000029</v>
       </c>
       <c r="F268">
-        <v>0.56000000000000028</v>
+        <v>0.63000000000000034</v>
       </c>
       <c r="G268">
         <v>0.42000000000000015</v>
@@ -7151,12 +7146,10 @@
         <v>5.3061224489795915</v>
       </c>
       <c r="E269">
-        <f t="shared" ref="B269:M270" si="15">AVERAGE(E267:E268)</f>
         <v>0.70000000000000029</v>
       </c>
       <c r="F269">
-        <f t="shared" si="15"/>
-        <v>0.59500000000000031</v>
+        <v>0.56000000000000028</v>
       </c>
       <c r="G269">
         <v>0.70000000000000029</v>
@@ -7185,7 +7178,7 @@
         <v>27</v>
       </c>
       <c r="B270">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="B269:M270" si="15">AVERAGE(B268:B269)</f>
         <v>3.8775510204081631</v>
       </c>
       <c r="C270">
@@ -7197,12 +7190,12 @@
         <v>5.3061224489795915</v>
       </c>
       <c r="E270">
-        <f t="shared" ref="B270:M271" si="16">(SQRT(E263-1))*E269</f>
-        <v>0.98994949366116702</v>
+        <f>AVERAGE(E268:E269)</f>
+        <v>0.70000000000000029</v>
       </c>
       <c r="F270">
-        <f t="shared" si="16"/>
-        <v>0.84145706961199207</v>
+        <f>AVERAGE(F268:F269)</f>
+        <v>0.59500000000000031</v>
       </c>
       <c r="G270">
         <f t="shared" si="15"/>
@@ -7238,7 +7231,7 @@
         <v>25</v>
       </c>
       <c r="B271">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="B270:M271" si="16">(SQRT(B264-1))*B270</f>
         <v>5.4836852418548583</v>
       </c>
       <c r="C271">
@@ -7281,12 +7274,6 @@
     <row r="272" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A272" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="E272" t="s">
-        <v>89</v>
-      </c>
-      <c r="F272" t="s">
-        <v>14</v>
       </c>
       <c r="Y272" s="12"/>
       <c r="Z272" s="12"/>
@@ -7311,11 +7298,11 @@
       <c r="D273" t="s">
         <v>3</v>
       </c>
-      <c r="E273">
-        <v>3</v>
-      </c>
-      <c r="F273">
-        <v>3</v>
+      <c r="E273" t="s">
+        <v>89</v>
+      </c>
+      <c r="F273" t="s">
+        <v>14</v>
       </c>
       <c r="G273" t="s">
         <v>15</v>
@@ -7362,10 +7349,10 @@
         <v>3</v>
       </c>
       <c r="E274">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F274">
-        <v>3.4999999999999996</v>
+        <v>3</v>
       </c>
       <c r="G274">
         <v>3</v>
@@ -7412,10 +7399,10 @@
         <v>5.25</v>
       </c>
       <c r="E275">
-        <v>10.5</v>
+        <v>8</v>
       </c>
       <c r="F275">
-        <v>8</v>
+        <v>3.4999999999999996</v>
       </c>
       <c r="G275">
         <v>4.7499999999999991</v>
@@ -7462,12 +7449,10 @@
         <v>1</v>
       </c>
       <c r="E276">
-        <f t="shared" ref="B276:M277" si="17">AVERAGE(E274:E275)</f>
-        <v>9.25</v>
+        <v>10.5</v>
       </c>
       <c r="F276">
-        <f t="shared" si="17"/>
-        <v>5.75</v>
+        <v>8</v>
       </c>
       <c r="G276">
         <v>16.75</v>
@@ -7505,7 +7490,7 @@
         <v>0</v>
       </c>
       <c r="B277">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="B276:M277" si="17">AVERAGE(B275:B276)</f>
         <v>12.625</v>
       </c>
       <c r="C277">
@@ -7517,10 +7502,12 @@
         <v>3.125</v>
       </c>
       <c r="E277">
-        <v>2</v>
+        <f>AVERAGE(E275:E276)</f>
+        <v>9.25</v>
       </c>
       <c r="F277">
-        <v>0.74999999999999989</v>
+        <f>AVERAGE(F275:F276)</f>
+        <v>5.75</v>
       </c>
       <c r="G277">
         <f t="shared" si="17"/>
@@ -7574,10 +7561,10 @@
         <v>4.5</v>
       </c>
       <c r="E278">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="F278">
-        <v>1.4999999999999998</v>
+        <v>0.74999999999999989</v>
       </c>
       <c r="G278">
         <v>0.74999999999999989</v>
@@ -7624,12 +7611,10 @@
         <v>0.5</v>
       </c>
       <c r="E279">
-        <f t="shared" ref="B279:M280" si="18">AVERAGE(E277:E278)</f>
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="F279">
-        <f t="shared" si="18"/>
-        <v>1.1249999999999998</v>
+        <v>1.4999999999999998</v>
       </c>
       <c r="G279">
         <v>3.75</v>
@@ -7667,7 +7652,7 @@
         <v>27</v>
       </c>
       <c r="B280">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="B279:M280" si="18">AVERAGE(B278:B279)</f>
         <v>3.3749999999999996</v>
       </c>
       <c r="C280">
@@ -7679,12 +7664,12 @@
         <v>2.5</v>
       </c>
       <c r="E280">
-        <f>(SQRT(E273-1))*E279</f>
-        <v>3.1819805153394642</v>
+        <f>AVERAGE(E278:E279)</f>
+        <v>2.25</v>
       </c>
       <c r="F280">
-        <f t="shared" si="18"/>
-        <v>1.3124999999999998</v>
+        <f>AVERAGE(F278:F279)</f>
+        <v>1.1249999999999998</v>
       </c>
       <c r="G280">
         <f t="shared" si="18"/>
@@ -7739,6 +7724,14 @@
       <c r="D281">
         <f>(SQRT(D274-1))*D280</f>
         <v>3.5355339059327378</v>
+      </c>
+      <c r="E281">
+        <f>(SQRT(E274-1))*E280</f>
+        <v>3.1819805153394642</v>
+      </c>
+      <c r="F281">
+        <f>AVERAGE(F279:F280)</f>
+        <v>1.3124999999999998</v>
       </c>
       <c r="G281">
         <f t="shared" ref="G281:M281" si="19">(SQRT(G274-1))*G280</f>
@@ -8066,12 +8059,6 @@
       </c>
       <c r="C296" s="6"/>
       <c r="D296" s="6"/>
-      <c r="E296" t="s">
-        <v>6</v>
-      </c>
-      <c r="F296" t="s">
-        <v>41</v>
-      </c>
       <c r="G296" s="6"/>
       <c r="H296" s="6"/>
       <c r="K296" s="6"/>
@@ -8106,11 +8093,11 @@
       <c r="D297" t="s">
         <v>4</v>
       </c>
-      <c r="E297">
+      <c r="E297" t="s">
         <v>6</v>
       </c>
-      <c r="F297">
-        <v>6</v>
+      <c r="F297" t="s">
+        <v>41</v>
       </c>
       <c r="G297" t="s">
         <v>9</v>
@@ -8154,10 +8141,10 @@
         <v>6</v>
       </c>
       <c r="E298">
-        <v>4.6276149999999996</v>
-      </c>
-      <c r="F298" s="6">
-        <v>0.41004184100000002</v>
+        <v>6</v>
+      </c>
+      <c r="F298">
+        <v>6</v>
       </c>
       <c r="G298">
         <v>6</v>
@@ -8200,11 +8187,11 @@
       <c r="D299">
         <v>2.635983264</v>
       </c>
-      <c r="E299" s="1">
-        <v>0.64435146399999998</v>
+      <c r="E299">
+        <v>4.6276149999999996</v>
       </c>
       <c r="F299" s="6">
-        <v>0.23430962299999999</v>
+        <v>0.41004184100000002</v>
       </c>
       <c r="G299" s="6">
         <v>1.9330543929999999</v>
@@ -8246,13 +8233,11 @@
       <c r="D300" s="1">
         <v>0.351464</v>
       </c>
-      <c r="E300">
-        <f t="shared" ref="D300:I301" si="20">(SQRT(E297-1))*E299</f>
-        <v>1.4408136749055085</v>
-      </c>
-      <c r="F300">
-        <f t="shared" si="20"/>
-        <v>0.52393224481034817</v>
+      <c r="E300" s="1">
+        <v>0.64435146399999998</v>
+      </c>
+      <c r="F300" s="6">
+        <v>0.23430962299999999</v>
       </c>
       <c r="G300" s="6">
         <v>0.29288702900000002</v>
@@ -8290,11 +8275,16 @@
         <v>2.7506442902854813</v>
       </c>
       <c r="D301">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="D300:I301" si="20">(SQRT(D298-1))*D300</f>
         <v>0.78589739564398609</v>
       </c>
       <c r="E301">
-        <v>4.1120999999999999</v>
+        <f>(SQRT(E298-1))*E300</f>
+        <v>1.4408136749055085</v>
+      </c>
+      <c r="F301">
+        <f>(SQRT(F298-1))*F300</f>
+        <v>0.52393224481034817</v>
       </c>
       <c r="G301">
         <f t="shared" si="20"/>
@@ -8332,7 +8322,7 @@
         <v>-0.3327</v>
       </c>
       <c r="E302">
-        <v>1.7161999999999999</v>
+        <v>4.1120999999999999</v>
       </c>
       <c r="G302">
         <v>2.5680999999999998</v>
@@ -8367,10 +8357,7 @@
         <v>94</v>
       </c>
       <c r="E303">
-        <v>6</v>
-      </c>
-      <c r="F303">
-        <v>6</v>
+        <v>1.7161999999999999</v>
       </c>
       <c r="H303" t="s">
         <v>1</v>
@@ -8411,11 +8398,11 @@
       <c r="D304">
         <v>6</v>
       </c>
-      <c r="E304" s="2">
-        <v>0.82008368200000004</v>
-      </c>
-      <c r="F304" s="3">
-        <v>0.175732218</v>
+      <c r="E304">
+        <v>6</v>
+      </c>
+      <c r="F304">
+        <v>6</v>
       </c>
       <c r="G304">
         <v>6</v>
@@ -8460,10 +8447,10 @@
         <v>0.29288702900000002</v>
       </c>
       <c r="E305" s="2">
-        <v>0.35146443500000002</v>
+        <v>0.82008368200000004</v>
       </c>
       <c r="F305" s="3">
-        <v>5.8577405999999999E-2</v>
+        <v>0.175732218</v>
       </c>
       <c r="G305" s="2">
         <v>3.1631799159999998</v>
@@ -8507,13 +8494,11 @@
       <c r="D306" s="2">
         <v>5.8577405999999999E-2</v>
       </c>
-      <c r="E306">
-        <f t="shared" ref="D306:I307" si="21">(SQRT(E303-1))*E305</f>
-        <v>0.78589836833355642</v>
-      </c>
-      <c r="F306">
-        <f t="shared" si="21"/>
-        <v>0.13098306176160404</v>
+      <c r="E306" s="2">
+        <v>0.35146443500000002</v>
+      </c>
+      <c r="F306" s="3">
+        <v>5.8577405999999999E-2</v>
       </c>
       <c r="G306" s="2">
         <v>1.9330543929999999</v>
@@ -8548,11 +8533,16 @@
         <v>3.0126104138086891</v>
       </c>
       <c r="D307">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="D306:I307" si="21">(SQRT(D304-1))*D306</f>
         <v>0.13098306176160404</v>
       </c>
       <c r="E307">
-        <v>0.93579999999999997</v>
+        <f>(SQRT(E304-1))*E306</f>
+        <v>0.78589836833355642</v>
+      </c>
+      <c r="F307">
+        <f>(SQRT(F304-1))*F306</f>
+        <v>0.13098306176160404</v>
       </c>
       <c r="G307">
         <f t="shared" si="21"/>
@@ -8583,6 +8573,9 @@
       </c>
       <c r="C308">
         <v>2.12E-2</v>
+      </c>
+      <c r="E308">
+        <v>0.93579999999999997</v>
       </c>
       <c r="G308">
         <v>0.97699999999999998</v>
@@ -9229,348 +9222,463 @@
         <v>19.595917942265423</v>
       </c>
     </row>
-    <row r="337" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A337" s="8"/>
     </row>
-    <row r="338" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A338" s="15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="339" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A339" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E339" t="s">
-        <v>12</v>
-      </c>
-      <c r="F339" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="340" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="340" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A340" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B340" t="s">
+      <c r="B340" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C340" t="s">
-        <v>3</v>
-      </c>
-      <c r="D340" t="s">
+      <c r="C340" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D340" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E340">
-        <v>3</v>
-      </c>
-      <c r="F340">
-        <v>3</v>
-      </c>
-      <c r="G340" t="s">
+      <c r="E340" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F340" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G340" s="12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="341" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="I340" t="s">
+        <v>63</v>
+      </c>
+      <c r="J340" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="341" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A341" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B341">
-        <v>3</v>
-      </c>
-      <c r="C341">
-        <v>3</v>
-      </c>
-      <c r="D341">
-        <v>3</v>
-      </c>
-      <c r="E341">
-        <v>6.5</v>
-      </c>
-      <c r="F341">
-        <v>1.5</v>
-      </c>
-      <c r="G341">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="342" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B341" s="12">
+        <v>3</v>
+      </c>
+      <c r="C341" s="12">
+        <v>3</v>
+      </c>
+      <c r="D341" s="12">
+        <v>3</v>
+      </c>
+      <c r="E341" s="12">
+        <v>3</v>
+      </c>
+      <c r="F341" s="12">
+        <v>3</v>
+      </c>
+      <c r="G341" s="12">
+        <v>3</v>
+      </c>
+      <c r="I341" s="12">
+        <v>3</v>
+      </c>
+      <c r="J341" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="342" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A342" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B342">
+      <c r="B342" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="C342" s="12">
         <v>12</v>
       </c>
-      <c r="C342">
-        <v>5.5</v>
-      </c>
-      <c r="D342">
-        <v>4.5</v>
-      </c>
-      <c r="E342">
-        <v>0.5</v>
-      </c>
-      <c r="F342">
-        <v>0.1</v>
-      </c>
-      <c r="G342">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="343" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="D342" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="E342" s="12">
+        <v>7.5</v>
+      </c>
+      <c r="F342" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="G342" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="I342" s="12">
+        <v>4</v>
+      </c>
+      <c r="J342" s="12">
+        <v>11</v>
+      </c>
+      <c r="L342">
+        <f>SQRT((D343^2)+(F343^2))</f>
+        <v>0.76157731058639078</v>
+      </c>
+      <c r="M342">
+        <f>SQRT((E343^2)+(G343^2))</f>
+        <v>0.58309518948452999</v>
+      </c>
+    </row>
+    <row r="343" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A343" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B343">
+      <c r="B343" s="12">
         <v>0.5</v>
       </c>
-      <c r="C343">
+      <c r="C343" s="12">
         <v>0.5</v>
       </c>
-      <c r="D343">
+      <c r="D343" s="12">
         <v>0.7</v>
       </c>
-      <c r="E343">
-        <f>(SQRT(E340-1))*D343</f>
-        <v>0.98994949366116658</v>
-      </c>
-      <c r="F343">
-        <f>(SQRT(F340-1))*G343</f>
-        <v>7.0710678118654766E-2</v>
-      </c>
-      <c r="G343">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="344" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E343" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="F343" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="G343" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="I343" s="12">
+        <v>0.76157731058639078</v>
+      </c>
+      <c r="J343" s="12">
+        <v>0.58309518948452999</v>
+      </c>
+    </row>
+    <row r="344" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A344" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B344">
-        <f>(SQRT(B341-1))*C343</f>
+      <c r="B344" s="12">
         <v>0.70710678118654757</v>
       </c>
-      <c r="C344">
-        <f>(SQRT(C341-1))*B343</f>
+      <c r="C344" s="12">
         <v>0.70710678118654757</v>
       </c>
-      <c r="D344">
-        <f>(SQRT(D341-1))*E342</f>
+      <c r="D344" s="12">
         <v>0.70710678118654757</v>
       </c>
-      <c r="G344">
-        <f>(SQRT(G341-1))*F342</f>
-        <v>0.14142135623730953</v>
-      </c>
-    </row>
-    <row r="345" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E344" s="12">
+        <v>0.98994949366116658</v>
+      </c>
+      <c r="F344" s="12">
+        <v>0.42426406871192851</v>
+      </c>
+      <c r="G344" s="12">
+        <v>0.42426406871192851</v>
+      </c>
+      <c r="I344" s="12">
+        <v>0.82462112512353203</v>
+      </c>
+      <c r="J344" s="12">
+        <v>1.0770329614269007</v>
+      </c>
+    </row>
+    <row r="345" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A345" s="8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="346" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B345" s="12"/>
+      <c r="C345" s="12"/>
+      <c r="D345" s="12"/>
+      <c r="E345" s="12"/>
+      <c r="F345" s="12"/>
+      <c r="G345" s="12"/>
+    </row>
+    <row r="346" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A346" s="10"/>
-    </row>
-    <row r="347" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B346" s="12"/>
+      <c r="C346" s="12"/>
+      <c r="D346" s="12"/>
+      <c r="E346" s="12"/>
+      <c r="F346" s="12"/>
+      <c r="G346" s="12"/>
+    </row>
+    <row r="347" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A347" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B347" t="s">
+      <c r="B347" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C347" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="348" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="C347" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D347" s="12"/>
+      <c r="E347" s="12"/>
+      <c r="F347" s="12"/>
+      <c r="G347" s="12"/>
+    </row>
+    <row r="348" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A348" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B348">
-        <v>3</v>
-      </c>
-      <c r="C348">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="349" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B348" s="12">
+        <v>3</v>
+      </c>
+      <c r="C348" s="12">
+        <v>3</v>
+      </c>
+      <c r="D348" s="12"/>
+      <c r="E348" s="12"/>
+      <c r="F348" s="12"/>
+      <c r="G348" s="12"/>
+    </row>
+    <row r="349" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A349" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B349">
+      <c r="B349" s="12">
+        <v>290</v>
+      </c>
+      <c r="C349" s="12">
         <v>340</v>
       </c>
-      <c r="C349">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="350" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="D349" s="12"/>
+      <c r="E349" s="12"/>
+      <c r="F349" s="12"/>
+      <c r="G349" s="12"/>
+    </row>
+    <row r="350" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A350" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B350">
+      <c r="B350" s="12">
+        <v>30</v>
+      </c>
+      <c r="C350" s="12">
         <v>25</v>
       </c>
-      <c r="C350">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="351" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D350" s="12"/>
+      <c r="E350" s="12"/>
+      <c r="F350" s="12"/>
+      <c r="G350" s="12"/>
+    </row>
+    <row r="351" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A351" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B351">
-        <f>(SQRT(B348-1))*B350</f>
+      <c r="B351" s="12">
+        <v>42.426406871192853</v>
+      </c>
+      <c r="C351" s="12">
         <v>35.355339059327378</v>
       </c>
-      <c r="C351">
-        <f>(SQRT(C348-1))*C350</f>
-        <v>42.426406871192853</v>
-      </c>
-    </row>
-    <row r="352" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D351" s="12"/>
+      <c r="E351" s="12"/>
+      <c r="F351" s="12"/>
+      <c r="G351" s="12"/>
+    </row>
+    <row r="352" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A352" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B352" s="11"/>
-      <c r="C352" s="11"/>
-    </row>
-    <row r="353" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B352" s="27"/>
+      <c r="C352" s="27"/>
+      <c r="D352" s="12"/>
+      <c r="E352" s="12"/>
+      <c r="F352" s="12"/>
+      <c r="G352" s="12"/>
+    </row>
+    <row r="353" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A353" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C353" s="11"/>
-      <c r="E353" t="s">
-        <v>12</v>
-      </c>
-      <c r="F353" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="354" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B353" s="12"/>
+      <c r="C353" s="27"/>
+      <c r="D353" s="12"/>
+      <c r="E353" s="12"/>
+      <c r="F353" s="12"/>
+      <c r="G353" s="12"/>
+    </row>
+    <row r="354" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A354" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B354" t="s">
+      <c r="B354" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C354" t="s">
-        <v>3</v>
-      </c>
-      <c r="D354" t="s">
+      <c r="C354" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D354" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E354">
-        <v>3</v>
-      </c>
-      <c r="F354">
-        <v>3</v>
-      </c>
-      <c r="G354" t="s">
+      <c r="E354" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F354" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G354" s="12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="355" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="I354" t="s">
+        <v>63</v>
+      </c>
+      <c r="J354" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="355" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A355" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B355">
-        <v>3</v>
-      </c>
-      <c r="C355">
-        <v>3</v>
-      </c>
-      <c r="D355">
-        <v>3</v>
-      </c>
-      <c r="E355">
-        <v>7</v>
-      </c>
-      <c r="F355">
-        <v>2</v>
-      </c>
-      <c r="G355">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="356" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B355" s="12">
+        <v>3</v>
+      </c>
+      <c r="C355" s="12">
+        <v>3</v>
+      </c>
+      <c r="D355" s="12">
+        <v>3</v>
+      </c>
+      <c r="E355" s="12">
+        <v>3</v>
+      </c>
+      <c r="F355" s="12">
+        <v>3</v>
+      </c>
+      <c r="G355" s="12">
+        <v>3</v>
+      </c>
+      <c r="I355" s="12">
+        <v>3</v>
+      </c>
+      <c r="J355" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="356" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A356" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B356">
+      <c r="B356" s="12">
         <v>5.3</v>
       </c>
-      <c r="C356">
+      <c r="C356" s="12">
         <v>5.3</v>
       </c>
-      <c r="D356">
+      <c r="D356" s="12">
+        <v>3</v>
+      </c>
+      <c r="E356" s="12">
+        <v>4</v>
+      </c>
+      <c r="F356" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="G356" s="12">
+        <v>1</v>
+      </c>
+      <c r="I356" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="J356" s="12">
         <v>5</v>
       </c>
-      <c r="E356">
-        <v>1</v>
-      </c>
-      <c r="F356">
-        <v>0.5</v>
-      </c>
-      <c r="G356">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="357" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="L356">
+        <f>SQRT((D357^2)+(F357^2))</f>
+        <v>0.58309518948452999</v>
+      </c>
+      <c r="M356">
+        <f>SQRT((E357^2)+(G357^2))</f>
+        <v>1.1180339887498949</v>
+      </c>
+    </row>
+    <row r="357" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A357" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B357">
+      <c r="B357" s="12">
         <v>2.5</v>
       </c>
-      <c r="C357">
+      <c r="C357" s="12">
         <v>2</v>
       </c>
-      <c r="D357">
+      <c r="D357" s="12">
         <v>0.5</v>
       </c>
-      <c r="E357">
-        <f t="shared" ref="B357:G358" si="24">(SQRT(E354-1))*E356</f>
-        <v>1.4142135623730951</v>
-      </c>
-      <c r="F357">
-        <f t="shared" si="24"/>
-        <v>0.70710678118654757</v>
-      </c>
-      <c r="G357">
+      <c r="E357" s="12">
+        <v>1</v>
+      </c>
+      <c r="F357" s="12">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="358" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G357" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="I357" s="12">
+        <v>0.58309518948452999</v>
+      </c>
+      <c r="J357" s="12">
+        <v>1.1180339887498949</v>
+      </c>
+    </row>
+    <row r="358" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A358" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B358">
-        <f t="shared" si="24"/>
+      <c r="B358" s="12">
         <v>3.5355339059327378</v>
       </c>
-      <c r="C358">
-        <f t="shared" si="24"/>
+      <c r="C358" s="12">
         <v>2.8284271247461903</v>
       </c>
-      <c r="D358">
-        <f t="shared" si="24"/>
+      <c r="D358" s="12">
         <v>0.70710678118654757</v>
       </c>
-      <c r="G358">
-        <f t="shared" si="24"/>
+      <c r="E358" s="12">
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="F358" s="12">
         <v>0.42426406871192851</v>
       </c>
-    </row>
-    <row r="359" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G358" s="12">
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="I358" s="12">
+        <v>1.5811388300841898</v>
+      </c>
+      <c r="J358" s="12">
+        <v>0.82462112512353203</v>
+      </c>
+    </row>
+    <row r="359" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A359" s="8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="360" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B359" s="12"/>
+      <c r="C359" s="12"/>
+      <c r="D359" s="12"/>
+      <c r="E359" s="12"/>
+      <c r="F359" s="12"/>
+      <c r="G359" s="12"/>
+    </row>
+    <row r="360" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A360" s="10"/>
-    </row>
-    <row r="361" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B360" s="12"/>
+      <c r="C360" s="12"/>
+      <c r="D360" s="12"/>
+      <c r="E360" s="12"/>
+      <c r="F360" s="12"/>
+      <c r="G360" s="12"/>
+    </row>
+    <row r="361" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A361" s="8" t="s">
         <v>32</v>
       </c>
@@ -9581,7 +9689,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="362" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A362" s="10" t="s">
         <v>26</v>
       </c>
@@ -9592,7 +9700,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="363" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A363" s="10" t="s">
         <v>0</v>
       </c>
@@ -9603,7 +9711,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="364" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A364" s="10" t="s">
         <v>27</v>
       </c>
@@ -9614,42 +9722,37 @@
         <v>50</v>
       </c>
     </row>
-    <row r="365" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A365" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B365">
-        <f>(SQRT(B362-1))*B364</f>
         <v>42.426406871192853</v>
       </c>
       <c r="C365">
-        <f>(SQRT(C362-1))*C364</f>
         <v>70.710678118654755</v>
       </c>
-      <c r="E365" s="6"/>
-    </row>
-    <row r="366" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="366" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A366" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B366" s="11"/>
       <c r="D366" s="6"/>
       <c r="E366" s="6"/>
-      <c r="F366" s="6"/>
-    </row>
-    <row r="367" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="367" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A367" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C367" s="6"/>
       <c r="D367" s="6"/>
-      <c r="E367" t="s">
-        <v>14</v>
-      </c>
+      <c r="E367" s="6"/>
+      <c r="F367" s="6"/>
       <c r="G367" s="6"/>
       <c r="H367" s="6"/>
     </row>
-    <row r="368" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A368" s="4" t="s">
         <v>30</v>
       </c>
@@ -9662,8 +9765,8 @@
       <c r="D368" t="s">
         <v>89</v>
       </c>
-      <c r="E368">
-        <v>3</v>
+      <c r="E368" t="s">
+        <v>14</v>
       </c>
       <c r="J368" s="2"/>
     </row>
@@ -9680,10 +9783,9 @@
       <c r="D369">
         <v>3</v>
       </c>
-      <c r="E369" s="2">
-        <v>11</v>
-      </c>
-      <c r="F369" s="3"/>
+      <c r="E369">
+        <v>3</v>
+      </c>
       <c r="J369" s="3"/>
     </row>
     <row r="370" spans="1:13" ht="15" x14ac:dyDescent="0.25">
@@ -9700,7 +9802,7 @@
         <v>9</v>
       </c>
       <c r="E370" s="2">
-        <v>4.4000000000000004</v>
+        <v>11</v>
       </c>
       <c r="F370" s="3"/>
       <c r="G370" s="2"/>
@@ -9724,10 +9826,10 @@
       <c r="D371" s="2">
         <v>8.6999999999999993</v>
       </c>
-      <c r="E371">
-        <f>(SQRT(E368-1))*E370</f>
-        <v>6.2225396744416193</v>
-      </c>
+      <c r="E371" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F371" s="3"/>
       <c r="G371" s="2"/>
       <c r="H371" s="3"/>
       <c r="I371" s="6"/>
@@ -9749,6 +9851,10 @@
         <f>(SQRT(D369-1))*D371</f>
         <v>12.303657992645928</v>
       </c>
+      <c r="E372">
+        <f>(SQRT(E369-1))*E371</f>
+        <v>6.2225396744416193</v>
+      </c>
       <c r="J372" s="2"/>
     </row>
     <row r="373" spans="1:13" ht="15" x14ac:dyDescent="0.25">
@@ -10264,12 +10370,6 @@
         <v>104</v>
       </c>
       <c r="C409" s="6"/>
-      <c r="E409" t="s">
-        <v>63</v>
-      </c>
-      <c r="F409" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="410" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A410" s="4" t="s">
@@ -10284,11 +10384,11 @@
       <c r="D410" t="s">
         <v>3</v>
       </c>
-      <c r="E410">
-        <v>3</v>
-      </c>
-      <c r="F410">
-        <v>3</v>
+      <c r="E410" t="s">
+        <v>63</v>
+      </c>
+      <c r="F410" t="s">
+        <v>43</v>
       </c>
       <c r="G410" t="s">
         <v>97</v>
@@ -10307,11 +10407,11 @@
       <c r="D411">
         <v>3</v>
       </c>
-      <c r="E411" s="22">
-        <v>3.3</v>
-      </c>
-      <c r="F411" s="6">
-        <v>3.3</v>
+      <c r="E411">
+        <v>3</v>
+      </c>
+      <c r="F411">
+        <v>3</v>
       </c>
       <c r="G411">
         <v>3</v>
@@ -10331,10 +10431,10 @@
         <v>11.6</v>
       </c>
       <c r="E412" s="22">
-        <v>0.2</v>
+        <v>3.3</v>
       </c>
       <c r="F412" s="6">
-        <v>0.2</v>
+        <v>3.25</v>
       </c>
       <c r="G412" s="2">
         <v>5.0999999999999996</v>
@@ -10353,19 +10453,17 @@
       <c r="D413" s="2">
         <v>0.2</v>
       </c>
-      <c r="E413">
-        <f>(SQRT(E410-1))*E412</f>
-        <v>0.28284271247461906</v>
-      </c>
-      <c r="F413">
-        <f>(SQRT(F410-1))*F412</f>
-        <v>0.28284271247461906</v>
+      <c r="E413" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="F413" s="6">
+        <v>0.2</v>
       </c>
       <c r="G413" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row r="414" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A414" s="4" t="s">
         <v>25</v>
       </c>
@@ -10381,7 +10479,14 @@
         <f>(SQRT(D411-1))*D413</f>
         <v>0.28284271247461906</v>
       </c>
-      <c r="E414" s="1"/>
+      <c r="E414">
+        <f>(SQRT(E411-1))*E413</f>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="F414">
+        <f>(SQRT(F411-1))*F413</f>
+        <v>0.28284271247461906</v>
+      </c>
       <c r="G414">
         <f>(SQRT(G411-1))*G413</f>
         <v>0.56568542494923812</v>
@@ -10896,7 +11001,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="E446">
-        <f t="shared" ref="C446:E447" si="25">(SQRT(E443-1))*E445</f>
+        <f t="shared" ref="C446:E447" si="24">(SQRT(E443-1))*E445</f>
         <v>0</v>
       </c>
       <c r="F446">
@@ -10916,11 +11021,11 @@
         <v>0</v>
       </c>
       <c r="C447">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="D447">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="E447" t="s">
@@ -10996,7 +11101,7 @@
         <v>0</v>
       </c>
       <c r="E451">
-        <f t="shared" ref="C451:E452" si="26">(SQRT(E448-1))*E450</f>
+        <f t="shared" ref="C451:E452" si="25">(SQRT(E448-1))*E450</f>
         <v>0</v>
       </c>
     </row>
@@ -11009,11 +11114,11 @@
         <v>0</v>
       </c>
       <c r="C452">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="D452">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
@@ -11748,7 +11853,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId4" name="Control 2">
+        <control shapeId="1025" r:id="rId4" name="Control 1">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
@@ -11759,21 +11864,21 @@
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>190500</xdr:colOff>
-                <xdr:row>102</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>103</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId4" name="Control 2"/>
+        <control shapeId="1025" r:id="rId4" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId6" name="Control 1">
+        <control shapeId="1026" r:id="rId6" name="Control 2">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
@@ -11784,16 +11889,16 @@
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>190500</xdr:colOff>
-                <xdr:row>102</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>103</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId6" name="Control 1"/>
+        <control shapeId="1026" r:id="rId6" name="Control 2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>